<commit_message>
start at web service
</commit_message>
<xml_diff>
--- a/test/resources/unittest_DAZHO_1.xlsx
+++ b/test/resources/unittest_DAZHO_1.xlsx
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>Decrees, reports, a message of spiritual consistory, requests, communication of church ministers. Diocese of church lands of diocese</t>
+          <t>Decrees, reports, reports of the spiritual consistory, request, communication of church ministers. Diocese of church lands diocese</t>
         </is>
       </c>
       <c r="C10" s="25" t="inlineStr">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="B22" s="5" t="inlineStr">
         <is>
-          <t>Decrees, disposal of spiritual consistory, business cases in the diocesan administration, cases of church lands. The case of the construction and repair of churches in the Volyn Diocese. Decrees of the Synod, the Senate, the order of the Consistory. Reports, the message of spiritual boards. DEPARTMENTS ABOUT COLLECTIVE ACTIVITIES AND PUPILS</t>
+          <t>Decrees, disposal of spiritual consistory, business cases in the diocesan administration, cases of church lands. The case of the construction and repair of churches in the Volyn Diocese. Decrees of the Synod, the Senate, the order of the Consistory. Reports, the message of spiritual boards. DEPARTMENTS ABOUT COLLECTIONS AND CULSIFIALS</t>
         </is>
       </c>
       <c r="C22" s="25" t="inlineStr">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. The case of the foundation of the Kremenets Epiphany Feast of the Nikolaev Brotherhood (c. 33)</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. The case of the founding of the Kremenets Epiphany Feast of the Nikolaev Brotherhood (c. 33)</t>
         </is>
       </c>
       <c r="C28" s="25" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. On the issuance of metric certificates. Information about churches was built in the Volyn Diocese in 1883. (cf. 6). About persons annexed to Orthodoxy in 1883, 1887. (Spr. 7: 56). Cases about the personnel of the monasteries of the Volyn Diocese</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. On the issuance of metric certificates. Information about the churches was built in the Volyn Diocese in 1883. (cf. 6). About persons annexed to Orthodoxy in 1883, 1887. (Spr. 7: 56). Cases about the personnel of the monasteries of the Volyn Diocese</t>
         </is>
       </c>
       <c r="C29" s="25" t="inlineStr">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. Cases about Church Parcels and Bogodil (Spr. 125), Church Century and Brotherhood (Spr. 60)</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. Cases about Church Primary Hospitals and Bogodil (Ref. 125), Church Hands and Brotherhood (Spr. 60)</t>
         </is>
       </c>
       <c r="C34" s="25" t="inlineStr">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="B40" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. The case of persons annexed to Orthodoxy for 1905 (file 25: 68). About Church-Parish Parishioners and Brotherhoods (Ref. 339), Bogodil (Ref. 338), libraries, (file 417) for 1905 on the spiritual and concern institutions and church-parish schools in 1905 (file 476). On the opening of church -parish fraternities at the churches of Dubno (c. 892), p. Stoke of Kovel County (Ref. 1382)</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. The case of persons annexed to Orthodoxy for 1905 (file 25: 68). About Church Parish Care and Brotherhood (Ref. 339), Bogodilny (Ref. 338), libraries, (file 417) for 1905 on spiritual and concern institutions and church-parish schools in 1905 (file 476). On the opening of church -parish fraternities at the churches of Dubno (c. 892), p. Stoke of Kovel County (Ref. 1382)</t>
         </is>
       </c>
       <c r="C40" s="25" t="inlineStr">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t>Cases of the appointment, movement, awarding and dismissal of church ministers. On the issuance of metric certificates. On the opening of church -parish brotherhoods in the village. Kremenchuk Zaslavsky County (file 4), Novograd-Volynskyi (Ref. 1462). About persons annexed to Orthodoxy in 1906. (cf. 70). Information on Church Parish Care and Brotherhood for 1906 (Ref. 299)</t>
+          <t>Cases of the appointment, movement, awarding and release of church ministers. On the issuance of metric certificates. On the opening of church -parish brotherhoods in the village. Kremenchuk Zaslavsky County (file 4), Novograd-Volynskyi (Ref. 1462). About persons annexed to Orthodoxy in 1906. (cf. 70). Information on Church Parish Care and Brotherhood for 1906 (Ref. 299)</t>
         </is>
       </c>
       <c r="C41" s="25" t="inlineStr">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>Cases of the appointment, movement, awarding and dismissal of church ministers. About persons annexed to Orthodoxy in 1907. (cf. 39). The case of opening in Zhytomyr school of pastoralism (file 1565)</t>
+          <t>Cases of the appointment, movement, awarding and release of church ministers. About persons annexed to Orthodoxy in 1907. (cf. 39). The case of opening in Zhytomyr school of pastoralism (file 1565)</t>
         </is>
       </c>
       <c r="C42" s="25" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>Cases about the appointment, movement and release of church ministers. Cases of Issuing Metric Certificates, Adoption, Division of Marriages</t>
+          <t>Cases about the appointment, movement and release of church ministers. Cases about the issuance of metric certificates, adoption, termination of marriage</t>
         </is>
       </c>
       <c r="C43" s="25" t="inlineStr">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="B44" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. DEPARTMENTS ABOUT COLLECTIONS AND CULSIFIALS</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. DEPARTMENTS ABOUT COLLECTIONS AND CULSE</t>
         </is>
       </c>
       <c r="C44" s="25" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>Cases of the appointment, movement, awarding and dismissal of church ministers. About persons annexed to Orthodoxy (file 1). About the opening of the Orthodox Czech Brotherhood (cf. 528)</t>
+          <t>Cases of the appointment, movement, awarding and release of church ministers. About persons annexed to Orthodoxy (file 1). About the opening of the Orthodox Czech Brotherhood (cf. 528)</t>
         </is>
       </c>
       <c r="C49" s="25" t="inlineStr">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="B51" s="5" t="inlineStr">
         <is>
-          <t>Cases of the appointment, movement, awarding and dismissal of priests and clergy. About persons annexed to Orthodoxy (Sf. 20)</t>
+          <t>Cases of the appointment, movement, awarding and dismissal of priests and clergy. About persons attached to Orthodoxy (Sf. 20)</t>
         </is>
       </c>
       <c r="C51" s="25" t="inlineStr">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="B62" s="5" t="inlineStr">
         <is>
-          <t>Annual reports on the course of insurance in the diocese. On the assessment and revaluation of church buildings subject to compulsory insurance. Information on the receipt and expenditure of insurance sums. Cases of compensation for damages from fires to the church tracts of the Volyn Diocese. About the appointment of charity and priests of the Diocese of Rewards for Labor for Insurance of Church Office buildings</t>
+          <t>Annual reports on the course of insurance in the diocese. On the assessment and revaluation of church buildings subject to compulsory insurance. Information on the receipt and expenditure of insurance sums. Cases of compensation for damages from fires to the church tracts of the Volyn Diocese. About the appointment of charity and priests of the Diocese of remuneration for work on insurance of the buildings of the church department</t>
         </is>
       </c>
       <c r="C62" s="25" t="inlineStr">
@@ -3694,7 +3694,7 @@
       </c>
       <c r="B66" s="5" t="inlineStr">
         <is>
-          <t>Annual reports on the course of Vetarchy insurance. On the assessment and revaluation of church buildings subject to compulsory insurance. Information on the receipt and expenditure of insurance sums. Cases of damages from fires to the church surroundings</t>
+          <t>Annual reports on the course of Vetarchy insurance. On the assessment and revaluation of church buildings subject to compulsory insurance. Information on the receipt and expenditure of insurance sums. Cases of damages from fires to the ecclesiastical surrender</t>
         </is>
       </c>
       <c r="C66" s="25" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B67" s="5" t="inlineStr">
         <is>
-          <t>Annual reports on the course of Vetarchy insurance. On the assessment and revaluation of church buildings subject to compulsory insurance. Information on the receipt and expenditure of insurance sums. Cases of damages from fires to the church surroundings</t>
+          <t>Annual reports on the course of Vetarchy insurance. On the assessment and revaluation of church buildings subject to compulsory insurance. Information on the receipt and expenditure of insurance sums. Cases of damages from fires to the ecclesiastical surrender</t>
         </is>
       </c>
       <c r="C67" s="25" t="inlineStr">
@@ -3964,7 +3964,7 @@
       </c>
       <c r="B72" s="5" t="inlineStr">
         <is>
-          <t>On the issuance of powers to the courts in courts of claim for the seizure of joint lands, felling of church forests, grass of fields and pastures, etc. The cases of peasants' complaints about priests and clergymen for the devastation of church forests. Cases on the exchange of church and peasant lands, leasing plots of church land. About the construction and repair of churches, the removal of places for new cemeteries and the expansion of existing cemeteries. On the opening of independent parishes. The case of repair and painting of the Cathedral Church in Starokostiantyniv (c. 117). On granting permits for the construction of roadside crosses and monuments. The case of a donation of Countess AA Grabbe Pochayiv Lavra sections of land for the construction of a monument temple (ref. 22). About donations by peasants with. Gladkovichi Ovruch County of Earth in X. Buda Lyar Ovruch St. Basil Monastery (Ref. 33)</t>
+          <t>On the issuance of powers to the courts in courts of claim for the seizure of joint lands, felling of church forests, grass of fields and pastures, etc. The cases of peasants' complaints about priests and clergymen for the devastation of church forests. Cases on the exchange of church and peasant lands, leasing plots of church land. About the construction and repair of churches, the removal of places for new cemeteries and the expansion of existing cemeteries. On the opening of independent parishes. The case of repair and painting of the Cathedral Church in Starokostiantyniv (c. 117). On granting permits for the construction of roadside crosses and monuments. The case of a donation of Countess AA Grabbe Pochaevskaya Lavra sections of land for the construction of a monument temple (ref. 22). About donations by peasants with. Gladkovichi Ovruch County of Earth in X. Buda Lyar Ovruch St. Basil Monastery (Ref. 33)</t>
         </is>
       </c>
       <c r="C72" s="25" t="inlineStr">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="B78" s="5" t="inlineStr">
         <is>
-          <t>Cases of the Zhidychyn Administrative Commission. On the collection of the tinting of the Basilian monasteries of fundamental sums and other payments provided on the estates of the landlords. Information about liquidated Basilian monasteries and their estates</t>
+          <t>Cases of the Zhidychyn Administrative Commission. On the collection of the tinting of the Basilian monasteries of the substitute amounts and other payments provided on the estates of the landlords. Information about liquidated Basilian monasteries and their estates</t>
         </is>
       </c>
       <c r="C78" s="25" t="inlineStr">
@@ -4459,7 +4459,7 @@
       </c>
       <c r="B83" s="5" t="inlineStr">
         <is>
-          <t>Metric books of Zhytomyr, Ovruch, Novograd-Volynsky, Radomysl, Skvyrsky, Berdychiv counties</t>
+          <t>Metric books of Zhytomyr, Ovruch, Novograd-Volyn, Radomysl, Skvyrsky, Berdychiv counties</t>
         </is>
       </c>
       <c r="C83" s="25" t="inlineStr">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="B88" s="5" t="inlineStr">
         <is>
-          <t>Description of cases and information about churches and priests of Radomysl county. Cases about the appointment of priests. On the consolidation of lands and lands on churches. Metric books of the church of the village. Ivanne Dubensky County for 1882 and churches of the village. Bortkovo, Vladimir's Bulk for 1830. The case of opening in Ostroh, the Diocesan Theological Seminary</t>
+          <t>Description of cases and information about churches and priests of Radomysl county. Cases about the appointment of priests. On the consolidation of lands and lands on churches. Metric books of the church of the village. Ivanne Dubensky County for 1882 and churches of the village. Bortkovo Vladimir Bait for 1830. The case of opening in Ostroh, the Diocesan Theological Seminary</t>
         </is>
       </c>
       <c r="C88" s="25" t="inlineStr">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="B89" s="5" t="inlineStr">
         <is>
-          <t>Metric books of Zhytomyr, Kremenetsky, Dubensky, Starokostiantynivsky, Zaslavsky, Novograd-Volynsky, Rivne, Ovruch, Ostroh counties. The Income Books of the Diocese Churches</t>
+          <t>Metric books of Zhytomyr, Kremenetsky, Dubensky, Starokostiantynivsky, Zaslavsky, Novograd-Volyn, Rivne, Ovruch, Ostroh counties. The Income Books of the Diocese Churches</t>
         </is>
       </c>
       <c r="C89" s="25" t="inlineStr">

</xml_diff>

<commit_message>
birddog webapp up and running
</commit_message>
<xml_diff>
--- a/test/resources/unittest_DAZHO_1.xlsx
+++ b/test/resources/unittest_DAZHO_1.xlsx
@@ -1007,56 +1007,16 @@
           <t>1790–1799</t>
         </is>
       </c>
-      <c r="D7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="E7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="F7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="G7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="H7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="I7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="J7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="K7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="L7" s="24" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
-      <c r="M7" s="27" t="inlineStr">
-        <is>
-          <t>{col}</t>
-        </is>
-      </c>
+      <c r="D7" s="24" t="inlineStr"/>
+      <c r="E7" s="24" t="inlineStr"/>
+      <c r="F7" s="24" t="inlineStr"/>
+      <c r="G7" s="24" t="inlineStr"/>
+      <c r="H7" s="24" t="inlineStr"/>
+      <c r="I7" s="24" t="inlineStr"/>
+      <c r="J7" s="24" t="inlineStr"/>
+      <c r="K7" s="24" t="inlineStr"/>
+      <c r="L7" s="24" t="inlineStr"/>
+      <c r="M7" s="27" t="inlineStr"/>
       <c r="N7" s="1" t="n"/>
       <c r="O7" s="1" t="n"/>
       <c r="P7" s="1" t="n"/>
@@ -1092,16 +1052,16 @@
           <t>1800–1805</t>
         </is>
       </c>
-      <c r="D8" s="24" t="n"/>
-      <c r="E8" s="24" t="n"/>
-      <c r="F8" s="24" t="n"/>
-      <c r="G8" s="24" t="n"/>
-      <c r="H8" s="24" t="n"/>
-      <c r="I8" s="24" t="n"/>
-      <c r="J8" s="24" t="n"/>
-      <c r="K8" s="24" t="n"/>
-      <c r="L8" s="24" t="n"/>
-      <c r="M8" s="27" t="n"/>
+      <c r="D8" s="24" t="inlineStr"/>
+      <c r="E8" s="24" t="inlineStr"/>
+      <c r="F8" s="24" t="inlineStr"/>
+      <c r="G8" s="24" t="inlineStr"/>
+      <c r="H8" s="24" t="inlineStr"/>
+      <c r="I8" s="24" t="inlineStr"/>
+      <c r="J8" s="24" t="inlineStr"/>
+      <c r="K8" s="24" t="inlineStr"/>
+      <c r="L8" s="24" t="inlineStr"/>
+      <c r="M8" s="27" t="inlineStr"/>
       <c r="N8" s="1" t="n"/>
       <c r="O8" s="1" t="n"/>
       <c r="P8" s="1" t="n"/>
@@ -1137,7 +1097,7 @@
           <t>1806–1812</t>
         </is>
       </c>
-      <c r="D9" s="24" t="n"/>
+      <c r="D9" s="24" t="inlineStr"/>
       <c r="E9" s="24" t="inlineStr"/>
       <c r="F9" s="24" t="inlineStr"/>
       <c r="G9" s="24" t="inlineStr"/>
@@ -1146,7 +1106,7 @@
       <c r="J9" s="24" t="inlineStr"/>
       <c r="K9" s="24" t="inlineStr"/>
       <c r="L9" s="24" t="inlineStr"/>
-      <c r="M9" s="27" t="n"/>
+      <c r="M9" s="27" t="inlineStr"/>
       <c r="N9" s="1" t="n"/>
       <c r="O9" s="1" t="n"/>
       <c r="P9" s="1" t="n"/>
@@ -1182,16 +1142,16 @@
           <t>1813–1819</t>
         </is>
       </c>
-      <c r="D10" s="24" t="n"/>
-      <c r="E10" s="24" t="n"/>
-      <c r="F10" s="24" t="n"/>
-      <c r="G10" s="24" t="n"/>
-      <c r="H10" s="24" t="n"/>
-      <c r="I10" s="24" t="n"/>
-      <c r="J10" s="24" t="n"/>
-      <c r="K10" s="24" t="n"/>
-      <c r="L10" s="24" t="n"/>
-      <c r="M10" s="27" t="n"/>
+      <c r="D10" s="24" t="inlineStr"/>
+      <c r="E10" s="24" t="inlineStr"/>
+      <c r="F10" s="24" t="inlineStr"/>
+      <c r="G10" s="24" t="inlineStr"/>
+      <c r="H10" s="24" t="inlineStr"/>
+      <c r="I10" s="24" t="inlineStr"/>
+      <c r="J10" s="24" t="inlineStr"/>
+      <c r="K10" s="24" t="inlineStr"/>
+      <c r="L10" s="24" t="inlineStr"/>
+      <c r="M10" s="27" t="inlineStr"/>
       <c r="N10" s="1" t="n"/>
       <c r="O10" s="1" t="n"/>
       <c r="P10" s="1" t="n"/>
@@ -1227,16 +1187,16 @@
           <t>1820–1826</t>
         </is>
       </c>
-      <c r="D11" s="24" t="n"/>
-      <c r="E11" s="24" t="n"/>
-      <c r="F11" s="24" t="n"/>
-      <c r="G11" s="24" t="n"/>
-      <c r="H11" s="24" t="n"/>
-      <c r="I11" s="24" t="n"/>
-      <c r="J11" s="24" t="n"/>
-      <c r="K11" s="24" t="n"/>
-      <c r="L11" s="24" t="n"/>
-      <c r="M11" s="27" t="n"/>
+      <c r="D11" s="24" t="inlineStr"/>
+      <c r="E11" s="24" t="inlineStr"/>
+      <c r="F11" s="24" t="inlineStr"/>
+      <c r="G11" s="24" t="inlineStr"/>
+      <c r="H11" s="24" t="inlineStr"/>
+      <c r="I11" s="24" t="inlineStr"/>
+      <c r="J11" s="24" t="inlineStr"/>
+      <c r="K11" s="24" t="inlineStr"/>
+      <c r="L11" s="24" t="inlineStr"/>
+      <c r="M11" s="27" t="inlineStr"/>
       <c r="N11" s="1" t="n"/>
       <c r="O11" s="1" t="n"/>
       <c r="P11" s="1" t="n"/>
@@ -1272,16 +1232,16 @@
           <t>1827–1830</t>
         </is>
       </c>
-      <c r="D12" s="24" t="n"/>
-      <c r="E12" s="24" t="n"/>
-      <c r="F12" s="24" t="n"/>
-      <c r="G12" s="24" t="n"/>
-      <c r="H12" s="24" t="n"/>
-      <c r="I12" s="24" t="n"/>
-      <c r="J12" s="24" t="n"/>
-      <c r="K12" s="24" t="n"/>
-      <c r="L12" s="24" t="n"/>
-      <c r="M12" s="27" t="n"/>
+      <c r="D12" s="24" t="inlineStr"/>
+      <c r="E12" s="24" t="inlineStr"/>
+      <c r="F12" s="24" t="inlineStr"/>
+      <c r="G12" s="24" t="inlineStr"/>
+      <c r="H12" s="24" t="inlineStr"/>
+      <c r="I12" s="24" t="inlineStr"/>
+      <c r="J12" s="24" t="inlineStr"/>
+      <c r="K12" s="24" t="inlineStr"/>
+      <c r="L12" s="24" t="inlineStr"/>
+      <c r="M12" s="27" t="inlineStr"/>
       <c r="N12" s="1" t="n"/>
       <c r="O12" s="1" t="n"/>
       <c r="P12" s="1" t="n"/>
@@ -1317,16 +1277,16 @@
           <t>1831–1835</t>
         </is>
       </c>
-      <c r="D13" s="24" t="n"/>
-      <c r="E13" s="24" t="n"/>
-      <c r="F13" s="24" t="n"/>
-      <c r="G13" s="24" t="n"/>
-      <c r="H13" s="24" t="n"/>
-      <c r="I13" s="24" t="n"/>
-      <c r="J13" s="24" t="n"/>
-      <c r="K13" s="24" t="n"/>
-      <c r="L13" s="24" t="n"/>
-      <c r="M13" s="27" t="n"/>
+      <c r="D13" s="24" t="inlineStr"/>
+      <c r="E13" s="24" t="inlineStr"/>
+      <c r="F13" s="24" t="inlineStr"/>
+      <c r="G13" s="24" t="inlineStr"/>
+      <c r="H13" s="24" t="inlineStr"/>
+      <c r="I13" s="24" t="inlineStr"/>
+      <c r="J13" s="24" t="inlineStr"/>
+      <c r="K13" s="24" t="inlineStr"/>
+      <c r="L13" s="24" t="inlineStr"/>
+      <c r="M13" s="27" t="inlineStr"/>
       <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="n"/>
       <c r="P13" s="1" t="n"/>
@@ -1362,16 +1322,16 @@
           <t>1836–1839</t>
         </is>
       </c>
-      <c r="D14" s="24" t="n"/>
-      <c r="E14" s="24" t="n"/>
-      <c r="F14" s="24" t="n"/>
-      <c r="G14" s="24" t="n"/>
-      <c r="H14" s="24" t="n"/>
-      <c r="I14" s="24" t="n"/>
-      <c r="J14" s="24" t="n"/>
-      <c r="K14" s="24" t="n"/>
-      <c r="L14" s="24" t="n"/>
-      <c r="M14" s="27" t="n"/>
+      <c r="D14" s="24" t="inlineStr"/>
+      <c r="E14" s="24" t="inlineStr"/>
+      <c r="F14" s="24" t="inlineStr"/>
+      <c r="G14" s="24" t="inlineStr"/>
+      <c r="H14" s="24" t="inlineStr"/>
+      <c r="I14" s="24" t="inlineStr"/>
+      <c r="J14" s="24" t="inlineStr"/>
+      <c r="K14" s="24" t="inlineStr"/>
+      <c r="L14" s="24" t="inlineStr"/>
+      <c r="M14" s="27" t="inlineStr"/>
       <c r="N14" s="1" t="n"/>
       <c r="O14" s="1" t="n"/>
       <c r="P14" s="1" t="n"/>
@@ -1407,16 +1367,16 @@
           <t>1840–1842</t>
         </is>
       </c>
-      <c r="D15" s="24" t="n"/>
-      <c r="E15" s="24" t="n"/>
-      <c r="F15" s="24" t="n"/>
-      <c r="G15" s="24" t="n"/>
-      <c r="H15" s="24" t="n"/>
-      <c r="I15" s="24" t="n"/>
-      <c r="J15" s="24" t="n"/>
-      <c r="K15" s="24" t="n"/>
-      <c r="L15" s="24" t="n"/>
-      <c r="M15" s="27" t="n"/>
+      <c r="D15" s="24" t="inlineStr"/>
+      <c r="E15" s="24" t="inlineStr"/>
+      <c r="F15" s="24" t="inlineStr"/>
+      <c r="G15" s="24" t="inlineStr"/>
+      <c r="H15" s="24" t="inlineStr"/>
+      <c r="I15" s="24" t="inlineStr"/>
+      <c r="J15" s="24" t="inlineStr"/>
+      <c r="K15" s="24" t="inlineStr"/>
+      <c r="L15" s="24" t="inlineStr"/>
+      <c r="M15" s="27" t="inlineStr"/>
       <c r="N15" s="1" t="n"/>
       <c r="O15" s="1" t="n"/>
       <c r="P15" s="1" t="n"/>
@@ -1452,16 +1412,16 @@
           <t>1843–1844</t>
         </is>
       </c>
-      <c r="D16" s="24" t="n"/>
-      <c r="E16" s="24" t="n"/>
-      <c r="F16" s="24" t="n"/>
-      <c r="G16" s="24" t="n"/>
-      <c r="H16" s="24" t="n"/>
-      <c r="I16" s="24" t="n"/>
-      <c r="J16" s="24" t="n"/>
-      <c r="K16" s="24" t="n"/>
-      <c r="L16" s="24" t="n"/>
-      <c r="M16" s="27" t="n"/>
+      <c r="D16" s="24" t="inlineStr"/>
+      <c r="E16" s="24" t="inlineStr"/>
+      <c r="F16" s="24" t="inlineStr"/>
+      <c r="G16" s="24" t="inlineStr"/>
+      <c r="H16" s="24" t="inlineStr"/>
+      <c r="I16" s="24" t="inlineStr"/>
+      <c r="J16" s="24" t="inlineStr"/>
+      <c r="K16" s="24" t="inlineStr"/>
+      <c r="L16" s="24" t="inlineStr"/>
+      <c r="M16" s="27" t="inlineStr"/>
       <c r="N16" s="1" t="n"/>
       <c r="O16" s="1" t="n"/>
       <c r="P16" s="1" t="n"/>
@@ -1497,16 +1457,16 @@
           <t>1845–1847</t>
         </is>
       </c>
-      <c r="D17" s="24" t="n"/>
-      <c r="E17" s="24" t="n"/>
-      <c r="F17" s="24" t="n"/>
-      <c r="G17" s="24" t="n"/>
-      <c r="H17" s="24" t="n"/>
-      <c r="I17" s="24" t="n"/>
-      <c r="J17" s="24" t="n"/>
-      <c r="K17" s="24" t="n"/>
-      <c r="L17" s="24" t="n"/>
-      <c r="M17" s="27" t="n"/>
+      <c r="D17" s="24" t="inlineStr"/>
+      <c r="E17" s="24" t="inlineStr"/>
+      <c r="F17" s="24" t="inlineStr"/>
+      <c r="G17" s="24" t="inlineStr"/>
+      <c r="H17" s="24" t="inlineStr"/>
+      <c r="I17" s="24" t="inlineStr"/>
+      <c r="J17" s="24" t="inlineStr"/>
+      <c r="K17" s="24" t="inlineStr"/>
+      <c r="L17" s="24" t="inlineStr"/>
+      <c r="M17" s="27" t="inlineStr"/>
       <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="n"/>
       <c r="P17" s="1" t="n"/>
@@ -1542,16 +1502,16 @@
           <t>1848–1849</t>
         </is>
       </c>
-      <c r="D18" s="24" t="n"/>
-      <c r="E18" s="24" t="n"/>
-      <c r="F18" s="24" t="n"/>
-      <c r="G18" s="24" t="n"/>
-      <c r="H18" s="24" t="n"/>
-      <c r="I18" s="24" t="n"/>
-      <c r="J18" s="24" t="n"/>
-      <c r="K18" s="24" t="n"/>
-      <c r="L18" s="24" t="n"/>
-      <c r="M18" s="27" t="n"/>
+      <c r="D18" s="24" t="inlineStr"/>
+      <c r="E18" s="24" t="inlineStr"/>
+      <c r="F18" s="24" t="inlineStr"/>
+      <c r="G18" s="24" t="inlineStr"/>
+      <c r="H18" s="24" t="inlineStr"/>
+      <c r="I18" s="24" t="inlineStr"/>
+      <c r="J18" s="24" t="inlineStr"/>
+      <c r="K18" s="24" t="inlineStr"/>
+      <c r="L18" s="24" t="inlineStr"/>
+      <c r="M18" s="27" t="inlineStr"/>
       <c r="N18" s="1" t="n"/>
       <c r="O18" s="1" t="n"/>
       <c r="P18" s="1" t="n"/>
@@ -1587,16 +1547,16 @@
           <t>1850–1853</t>
         </is>
       </c>
-      <c r="D19" s="24" t="n"/>
-      <c r="E19" s="24" t="n"/>
-      <c r="F19" s="24" t="n"/>
-      <c r="G19" s="24" t="n"/>
-      <c r="H19" s="24" t="n"/>
-      <c r="I19" s="24" t="n"/>
-      <c r="J19" s="24" t="n"/>
-      <c r="K19" s="24" t="n"/>
-      <c r="L19" s="24" t="n"/>
-      <c r="M19" s="27" t="n"/>
+      <c r="D19" s="24" t="inlineStr"/>
+      <c r="E19" s="24" t="inlineStr"/>
+      <c r="F19" s="24" t="inlineStr"/>
+      <c r="G19" s="24" t="inlineStr"/>
+      <c r="H19" s="24" t="inlineStr"/>
+      <c r="I19" s="24" t="inlineStr"/>
+      <c r="J19" s="24" t="inlineStr"/>
+      <c r="K19" s="24" t="inlineStr"/>
+      <c r="L19" s="24" t="inlineStr"/>
+      <c r="M19" s="27" t="inlineStr"/>
       <c r="N19" s="1" t="n"/>
       <c r="O19" s="1" t="n"/>
       <c r="P19" s="1" t="n"/>
@@ -1632,16 +1592,16 @@
           <t>1854–1856</t>
         </is>
       </c>
-      <c r="D20" s="24" t="n"/>
-      <c r="E20" s="24" t="n"/>
-      <c r="F20" s="24" t="n"/>
-      <c r="G20" s="24" t="n"/>
-      <c r="H20" s="24" t="n"/>
-      <c r="I20" s="24" t="n"/>
-      <c r="J20" s="24" t="n"/>
-      <c r="K20" s="24" t="n"/>
-      <c r="L20" s="24" t="n"/>
-      <c r="M20" s="27" t="n"/>
+      <c r="D20" s="24" t="inlineStr"/>
+      <c r="E20" s="24" t="inlineStr"/>
+      <c r="F20" s="24" t="inlineStr"/>
+      <c r="G20" s="24" t="inlineStr"/>
+      <c r="H20" s="24" t="inlineStr"/>
+      <c r="I20" s="24" t="inlineStr"/>
+      <c r="J20" s="24" t="inlineStr"/>
+      <c r="K20" s="24" t="inlineStr"/>
+      <c r="L20" s="24" t="inlineStr"/>
+      <c r="M20" s="27" t="inlineStr"/>
       <c r="N20" s="1" t="n"/>
       <c r="O20" s="1" t="n"/>
       <c r="P20" s="1" t="n"/>
@@ -1677,16 +1637,16 @@
           <t>1857–1859</t>
         </is>
       </c>
-      <c r="D21" s="24" t="n"/>
-      <c r="E21" s="24" t="n"/>
-      <c r="F21" s="24" t="n"/>
-      <c r="G21" s="24" t="n"/>
-      <c r="H21" s="24" t="n"/>
-      <c r="I21" s="24" t="n"/>
-      <c r="J21" s="24" t="n"/>
-      <c r="K21" s="24" t="n"/>
-      <c r="L21" s="24" t="n"/>
-      <c r="M21" s="27" t="n"/>
+      <c r="D21" s="24" t="inlineStr"/>
+      <c r="E21" s="24" t="inlineStr"/>
+      <c r="F21" s="24" t="inlineStr"/>
+      <c r="G21" s="24" t="inlineStr"/>
+      <c r="H21" s="24" t="inlineStr"/>
+      <c r="I21" s="24" t="inlineStr"/>
+      <c r="J21" s="24" t="inlineStr"/>
+      <c r="K21" s="24" t="inlineStr"/>
+      <c r="L21" s="24" t="inlineStr"/>
+      <c r="M21" s="27" t="inlineStr"/>
       <c r="N21" s="1" t="n"/>
       <c r="O21" s="1" t="n"/>
       <c r="P21" s="1" t="n"/>
@@ -1722,16 +1682,16 @@
           <t>1857–1859</t>
         </is>
       </c>
-      <c r="D22" s="24" t="n"/>
-      <c r="E22" s="24" t="n"/>
-      <c r="F22" s="24" t="n"/>
-      <c r="G22" s="24" t="n"/>
-      <c r="H22" s="24" t="n"/>
-      <c r="I22" s="24" t="n"/>
-      <c r="J22" s="24" t="n"/>
-      <c r="K22" s="24" t="n"/>
-      <c r="L22" s="24" t="n"/>
-      <c r="M22" s="27" t="n"/>
+      <c r="D22" s="24" t="inlineStr"/>
+      <c r="E22" s="24" t="inlineStr"/>
+      <c r="F22" s="24" t="inlineStr"/>
+      <c r="G22" s="24" t="inlineStr"/>
+      <c r="H22" s="24" t="inlineStr"/>
+      <c r="I22" s="24" t="inlineStr"/>
+      <c r="J22" s="24" t="inlineStr"/>
+      <c r="K22" s="24" t="inlineStr"/>
+      <c r="L22" s="24" t="inlineStr"/>
+      <c r="M22" s="27" t="inlineStr"/>
       <c r="N22" s="1" t="n"/>
       <c r="O22" s="1" t="n"/>
       <c r="P22" s="1" t="n"/>
@@ -1767,16 +1727,16 @@
           <t>1863–1866</t>
         </is>
       </c>
-      <c r="D23" s="24" t="n"/>
-      <c r="E23" s="24" t="n"/>
-      <c r="F23" s="24" t="n"/>
-      <c r="G23" s="24" t="n"/>
-      <c r="H23" s="24" t="n"/>
-      <c r="I23" s="24" t="n"/>
-      <c r="J23" s="24" t="n"/>
-      <c r="K23" s="24" t="n"/>
-      <c r="L23" s="24" t="n"/>
-      <c r="M23" s="27" t="n"/>
+      <c r="D23" s="24" t="inlineStr"/>
+      <c r="E23" s="24" t="inlineStr"/>
+      <c r="F23" s="24" t="inlineStr"/>
+      <c r="G23" s="24" t="inlineStr"/>
+      <c r="H23" s="24" t="inlineStr"/>
+      <c r="I23" s="24" t="inlineStr"/>
+      <c r="J23" s="24" t="inlineStr"/>
+      <c r="K23" s="24" t="inlineStr"/>
+      <c r="L23" s="24" t="inlineStr"/>
+      <c r="M23" s="27" t="inlineStr"/>
       <c r="N23" s="1" t="n"/>
       <c r="O23" s="1" t="n"/>
       <c r="P23" s="1" t="n"/>
@@ -1812,16 +1772,16 @@
           <t>1867–1869</t>
         </is>
       </c>
-      <c r="D24" s="24" t="n"/>
-      <c r="E24" s="24" t="n"/>
-      <c r="F24" s="24" t="n"/>
-      <c r="G24" s="24" t="n"/>
-      <c r="H24" s="24" t="n"/>
-      <c r="I24" s="24" t="n"/>
-      <c r="J24" s="24" t="n"/>
-      <c r="K24" s="24" t="n"/>
-      <c r="L24" s="24" t="n"/>
-      <c r="M24" s="27" t="n"/>
+      <c r="D24" s="24" t="inlineStr"/>
+      <c r="E24" s="24" t="inlineStr"/>
+      <c r="F24" s="24" t="inlineStr"/>
+      <c r="G24" s="24" t="inlineStr"/>
+      <c r="H24" s="24" t="inlineStr"/>
+      <c r="I24" s="24" t="inlineStr"/>
+      <c r="J24" s="24" t="inlineStr"/>
+      <c r="K24" s="24" t="inlineStr"/>
+      <c r="L24" s="24" t="inlineStr"/>
+      <c r="M24" s="27" t="inlineStr"/>
       <c r="N24" s="1" t="n"/>
       <c r="O24" s="1" t="n"/>
       <c r="P24" s="1" t="n"/>
@@ -1857,16 +1817,16 @@
           <t>1870</t>
         </is>
       </c>
-      <c r="D25" s="24" t="n"/>
-      <c r="E25" s="24" t="n"/>
-      <c r="F25" s="24" t="n"/>
-      <c r="G25" s="24" t="n"/>
-      <c r="H25" s="24" t="n"/>
-      <c r="I25" s="24" t="n"/>
-      <c r="J25" s="24" t="n"/>
-      <c r="K25" s="24" t="n"/>
-      <c r="L25" s="24" t="n"/>
-      <c r="M25" s="27" t="n"/>
+      <c r="D25" s="24" t="inlineStr"/>
+      <c r="E25" s="24" t="inlineStr"/>
+      <c r="F25" s="24" t="inlineStr"/>
+      <c r="G25" s="24" t="inlineStr"/>
+      <c r="H25" s="24" t="inlineStr"/>
+      <c r="I25" s="24" t="inlineStr"/>
+      <c r="J25" s="24" t="inlineStr"/>
+      <c r="K25" s="24" t="inlineStr"/>
+      <c r="L25" s="24" t="inlineStr"/>
+      <c r="M25" s="27" t="inlineStr"/>
       <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
       <c r="P25" s="1" t="n"/>
@@ -1902,16 +1862,16 @@
           <t>1873–1875</t>
         </is>
       </c>
-      <c r="D26" s="24" t="n"/>
-      <c r="E26" s="24" t="n"/>
-      <c r="F26" s="24" t="n"/>
-      <c r="G26" s="24" t="n"/>
-      <c r="H26" s="24" t="n"/>
-      <c r="I26" s="24" t="n"/>
-      <c r="J26" s="24" t="n"/>
-      <c r="K26" s="24" t="n"/>
-      <c r="L26" s="24" t="n"/>
-      <c r="M26" s="27" t="n"/>
+      <c r="D26" s="24" t="inlineStr"/>
+      <c r="E26" s="24" t="inlineStr"/>
+      <c r="F26" s="24" t="inlineStr"/>
+      <c r="G26" s="24" t="inlineStr"/>
+      <c r="H26" s="24" t="inlineStr"/>
+      <c r="I26" s="24" t="inlineStr"/>
+      <c r="J26" s="24" t="inlineStr"/>
+      <c r="K26" s="24" t="inlineStr"/>
+      <c r="L26" s="24" t="inlineStr"/>
+      <c r="M26" s="27" t="inlineStr"/>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="n"/>
       <c r="P26" s="1" t="n"/>
@@ -1947,16 +1907,16 @@
           <t>1876–1879</t>
         </is>
       </c>
-      <c r="D27" s="24" t="n"/>
-      <c r="E27" s="24" t="n"/>
-      <c r="F27" s="24" t="n"/>
-      <c r="G27" s="24" t="n"/>
-      <c r="H27" s="24" t="n"/>
-      <c r="I27" s="24" t="n"/>
-      <c r="J27" s="24" t="n"/>
-      <c r="K27" s="24" t="n"/>
-      <c r="L27" s="24" t="n"/>
-      <c r="M27" s="27" t="n"/>
+      <c r="D27" s="24" t="inlineStr"/>
+      <c r="E27" s="24" t="inlineStr"/>
+      <c r="F27" s="24" t="inlineStr"/>
+      <c r="G27" s="24" t="inlineStr"/>
+      <c r="H27" s="24" t="inlineStr"/>
+      <c r="I27" s="24" t="inlineStr"/>
+      <c r="J27" s="24" t="inlineStr"/>
+      <c r="K27" s="24" t="inlineStr"/>
+      <c r="L27" s="24" t="inlineStr"/>
+      <c r="M27" s="27" t="inlineStr"/>
       <c r="N27" s="1" t="n"/>
       <c r="O27" s="1" t="n"/>
       <c r="P27" s="1" t="n"/>
@@ -1992,16 +1952,16 @@
           <t>1880–1883</t>
         </is>
       </c>
-      <c r="D28" s="24" t="n"/>
-      <c r="E28" s="24" t="n"/>
-      <c r="F28" s="24" t="n"/>
-      <c r="G28" s="24" t="n"/>
-      <c r="H28" s="24" t="n"/>
-      <c r="I28" s="24" t="n"/>
-      <c r="J28" s="24" t="n"/>
-      <c r="K28" s="24" t="n"/>
-      <c r="L28" s="24" t="n"/>
-      <c r="M28" s="27" t="n"/>
+      <c r="D28" s="24" t="inlineStr"/>
+      <c r="E28" s="24" t="inlineStr"/>
+      <c r="F28" s="24" t="inlineStr"/>
+      <c r="G28" s="24" t="inlineStr"/>
+      <c r="H28" s="24" t="inlineStr"/>
+      <c r="I28" s="24" t="inlineStr"/>
+      <c r="J28" s="24" t="inlineStr"/>
+      <c r="K28" s="24" t="inlineStr"/>
+      <c r="L28" s="24" t="inlineStr"/>
+      <c r="M28" s="27" t="inlineStr"/>
       <c r="N28" s="1" t="n"/>
       <c r="O28" s="1" t="n"/>
       <c r="P28" s="1" t="n"/>
@@ -2037,16 +1997,16 @@
           <t>1884–1888</t>
         </is>
       </c>
-      <c r="D29" s="24" t="n"/>
-      <c r="E29" s="24" t="n"/>
-      <c r="F29" s="24" t="n"/>
-      <c r="G29" s="24" t="n"/>
-      <c r="H29" s="24" t="n"/>
-      <c r="I29" s="24" t="n"/>
-      <c r="J29" s="24" t="n"/>
-      <c r="K29" s="24" t="n"/>
-      <c r="L29" s="24" t="n"/>
-      <c r="M29" s="27" t="n"/>
+      <c r="D29" s="24" t="inlineStr"/>
+      <c r="E29" s="24" t="inlineStr"/>
+      <c r="F29" s="24" t="inlineStr"/>
+      <c r="G29" s="24" t="inlineStr"/>
+      <c r="H29" s="24" t="inlineStr"/>
+      <c r="I29" s="24" t="inlineStr"/>
+      <c r="J29" s="24" t="inlineStr"/>
+      <c r="K29" s="24" t="inlineStr"/>
+      <c r="L29" s="24" t="inlineStr"/>
+      <c r="M29" s="27" t="inlineStr"/>
       <c r="N29" s="1" t="n"/>
       <c r="O29" s="1" t="n"/>
       <c r="P29" s="1" t="n"/>
@@ -2082,16 +2042,16 @@
           <t>1889–1892</t>
         </is>
       </c>
-      <c r="D30" s="24" t="n"/>
-      <c r="E30" s="24" t="n"/>
-      <c r="F30" s="24" t="n"/>
-      <c r="G30" s="24" t="n"/>
-      <c r="H30" s="24" t="n"/>
-      <c r="I30" s="24" t="n"/>
-      <c r="J30" s="24" t="n"/>
-      <c r="K30" s="24" t="n"/>
-      <c r="L30" s="24" t="n"/>
-      <c r="M30" s="27" t="n"/>
+      <c r="D30" s="24" t="inlineStr"/>
+      <c r="E30" s="24" t="inlineStr"/>
+      <c r="F30" s="24" t="inlineStr"/>
+      <c r="G30" s="24" t="inlineStr"/>
+      <c r="H30" s="24" t="inlineStr"/>
+      <c r="I30" s="24" t="inlineStr"/>
+      <c r="J30" s="24" t="inlineStr"/>
+      <c r="K30" s="24" t="inlineStr"/>
+      <c r="L30" s="24" t="inlineStr"/>
+      <c r="M30" s="27" t="inlineStr"/>
       <c r="N30" s="1" t="n"/>
       <c r="O30" s="1" t="n"/>
       <c r="P30" s="1" t="n"/>
@@ -2127,16 +2087,16 @@
           <t>1893–1897</t>
         </is>
       </c>
-      <c r="D31" s="24" t="n"/>
-      <c r="E31" s="24" t="n"/>
-      <c r="F31" s="24" t="n"/>
-      <c r="G31" s="24" t="n"/>
-      <c r="H31" s="24" t="n"/>
-      <c r="I31" s="24" t="n"/>
-      <c r="J31" s="24" t="n"/>
-      <c r="K31" s="24" t="n"/>
-      <c r="L31" s="24" t="n"/>
-      <c r="M31" s="27" t="n"/>
+      <c r="D31" s="24" t="inlineStr"/>
+      <c r="E31" s="24" t="inlineStr"/>
+      <c r="F31" s="24" t="inlineStr"/>
+      <c r="G31" s="24" t="inlineStr"/>
+      <c r="H31" s="24" t="inlineStr"/>
+      <c r="I31" s="24" t="inlineStr"/>
+      <c r="J31" s="24" t="inlineStr"/>
+      <c r="K31" s="24" t="inlineStr"/>
+      <c r="L31" s="24" t="inlineStr"/>
+      <c r="M31" s="27" t="inlineStr"/>
       <c r="N31" s="1" t="n"/>
       <c r="O31" s="1" t="n"/>
       <c r="P31" s="1" t="n"/>
@@ -2172,16 +2132,16 @@
           <t>1898</t>
         </is>
       </c>
-      <c r="D32" s="24" t="n"/>
-      <c r="E32" s="24" t="n"/>
-      <c r="F32" s="24" t="n"/>
-      <c r="G32" s="24" t="n"/>
-      <c r="H32" s="24" t="n"/>
-      <c r="I32" s="24" t="n"/>
-      <c r="J32" s="24" t="n"/>
-      <c r="K32" s="24" t="n"/>
-      <c r="L32" s="24" t="n"/>
-      <c r="M32" s="27" t="n"/>
+      <c r="D32" s="24" t="inlineStr"/>
+      <c r="E32" s="24" t="inlineStr"/>
+      <c r="F32" s="24" t="inlineStr"/>
+      <c r="G32" s="24" t="inlineStr"/>
+      <c r="H32" s="24" t="inlineStr"/>
+      <c r="I32" s="24" t="inlineStr"/>
+      <c r="J32" s="24" t="inlineStr"/>
+      <c r="K32" s="24" t="inlineStr"/>
+      <c r="L32" s="24" t="inlineStr"/>
+      <c r="M32" s="27" t="inlineStr"/>
       <c r="N32" s="1" t="n"/>
       <c r="O32" s="1" t="n"/>
       <c r="P32" s="1" t="n"/>
@@ -2217,16 +2177,16 @@
           <t>1899</t>
         </is>
       </c>
-      <c r="D33" s="24" t="n"/>
-      <c r="E33" s="24" t="n"/>
-      <c r="F33" s="24" t="n"/>
-      <c r="G33" s="24" t="n"/>
-      <c r="H33" s="24" t="n"/>
-      <c r="I33" s="24" t="n"/>
-      <c r="J33" s="24" t="n"/>
-      <c r="K33" s="24" t="n"/>
-      <c r="L33" s="24" t="n"/>
-      <c r="M33" s="27" t="n"/>
+      <c r="D33" s="24" t="inlineStr"/>
+      <c r="E33" s="24" t="inlineStr"/>
+      <c r="F33" s="24" t="inlineStr"/>
+      <c r="G33" s="24" t="inlineStr"/>
+      <c r="H33" s="24" t="inlineStr"/>
+      <c r="I33" s="24" t="inlineStr"/>
+      <c r="J33" s="24" t="inlineStr"/>
+      <c r="K33" s="24" t="inlineStr"/>
+      <c r="L33" s="24" t="inlineStr"/>
+      <c r="M33" s="27" t="inlineStr"/>
       <c r="N33" s="1" t="n"/>
       <c r="O33" s="1" t="n"/>
       <c r="P33" s="1" t="n"/>
@@ -2262,16 +2222,16 @@
           <t>1899</t>
         </is>
       </c>
-      <c r="D34" s="24" t="n"/>
-      <c r="E34" s="24" t="n"/>
-      <c r="F34" s="24" t="n"/>
-      <c r="G34" s="24" t="n"/>
-      <c r="H34" s="24" t="n"/>
-      <c r="I34" s="24" t="n"/>
-      <c r="J34" s="24" t="n"/>
-      <c r="K34" s="24" t="n"/>
-      <c r="L34" s="24" t="n"/>
-      <c r="M34" s="27" t="n"/>
+      <c r="D34" s="24" t="inlineStr"/>
+      <c r="E34" s="24" t="inlineStr"/>
+      <c r="F34" s="24" t="inlineStr"/>
+      <c r="G34" s="24" t="inlineStr"/>
+      <c r="H34" s="24" t="inlineStr"/>
+      <c r="I34" s="24" t="inlineStr"/>
+      <c r="J34" s="24" t="inlineStr"/>
+      <c r="K34" s="24" t="inlineStr"/>
+      <c r="L34" s="24" t="inlineStr"/>
+      <c r="M34" s="27" t="inlineStr"/>
       <c r="N34" s="1" t="n"/>
       <c r="O34" s="1" t="n"/>
       <c r="P34" s="1" t="n"/>
@@ -2307,16 +2267,16 @@
           <t>1901</t>
         </is>
       </c>
-      <c r="D35" s="24" t="n"/>
-      <c r="E35" s="24" t="n"/>
-      <c r="F35" s="24" t="n"/>
-      <c r="G35" s="24" t="n"/>
-      <c r="H35" s="24" t="n"/>
-      <c r="I35" s="24" t="n"/>
-      <c r="J35" s="24" t="n"/>
-      <c r="K35" s="24" t="n"/>
-      <c r="L35" s="24" t="n"/>
-      <c r="M35" s="27" t="n"/>
+      <c r="D35" s="24" t="inlineStr"/>
+      <c r="E35" s="24" t="inlineStr"/>
+      <c r="F35" s="24" t="inlineStr"/>
+      <c r="G35" s="24" t="inlineStr"/>
+      <c r="H35" s="24" t="inlineStr"/>
+      <c r="I35" s="24" t="inlineStr"/>
+      <c r="J35" s="24" t="inlineStr"/>
+      <c r="K35" s="24" t="inlineStr"/>
+      <c r="L35" s="24" t="inlineStr"/>
+      <c r="M35" s="27" t="inlineStr"/>
       <c r="N35" s="1" t="n"/>
       <c r="O35" s="1" t="n"/>
       <c r="P35" s="1" t="n"/>
@@ -2352,16 +2312,16 @@
           <t>1902</t>
         </is>
       </c>
-      <c r="D36" s="24" t="n"/>
-      <c r="E36" s="24" t="n"/>
-      <c r="F36" s="24" t="n"/>
-      <c r="G36" s="24" t="n"/>
-      <c r="H36" s="24" t="n"/>
-      <c r="I36" s="24" t="n"/>
-      <c r="J36" s="24" t="n"/>
-      <c r="K36" s="24" t="n"/>
-      <c r="L36" s="24" t="n"/>
-      <c r="M36" s="27" t="n"/>
+      <c r="D36" s="24" t="inlineStr"/>
+      <c r="E36" s="24" t="inlineStr"/>
+      <c r="F36" s="24" t="inlineStr"/>
+      <c r="G36" s="24" t="inlineStr"/>
+      <c r="H36" s="24" t="inlineStr"/>
+      <c r="I36" s="24" t="inlineStr"/>
+      <c r="J36" s="24" t="inlineStr"/>
+      <c r="K36" s="24" t="inlineStr"/>
+      <c r="L36" s="24" t="inlineStr"/>
+      <c r="M36" s="27" t="inlineStr"/>
       <c r="N36" s="1" t="n"/>
       <c r="O36" s="1" t="n"/>
       <c r="P36" s="1" t="n"/>
@@ -2397,16 +2357,16 @@
           <t>1903</t>
         </is>
       </c>
-      <c r="D37" s="24" t="n"/>
-      <c r="E37" s="24" t="n"/>
-      <c r="F37" s="24" t="n"/>
-      <c r="G37" s="24" t="n"/>
-      <c r="H37" s="24" t="n"/>
-      <c r="I37" s="24" t="n"/>
-      <c r="J37" s="24" t="n"/>
-      <c r="K37" s="24" t="n"/>
-      <c r="L37" s="24" t="n"/>
-      <c r="M37" s="27" t="n"/>
+      <c r="D37" s="24" t="inlineStr"/>
+      <c r="E37" s="24" t="inlineStr"/>
+      <c r="F37" s="24" t="inlineStr"/>
+      <c r="G37" s="24" t="inlineStr"/>
+      <c r="H37" s="24" t="inlineStr"/>
+      <c r="I37" s="24" t="inlineStr"/>
+      <c r="J37" s="24" t="inlineStr"/>
+      <c r="K37" s="24" t="inlineStr"/>
+      <c r="L37" s="24" t="inlineStr"/>
+      <c r="M37" s="27" t="inlineStr"/>
       <c r="N37" s="1" t="n"/>
       <c r="O37" s="1" t="n"/>
       <c r="P37" s="1" t="n"/>
@@ -2442,16 +2402,16 @@
           <t>1904</t>
         </is>
       </c>
-      <c r="D38" s="24" t="n"/>
-      <c r="E38" s="24" t="n"/>
-      <c r="F38" s="24" t="n"/>
-      <c r="G38" s="24" t="n"/>
-      <c r="H38" s="24" t="n"/>
-      <c r="I38" s="24" t="n"/>
-      <c r="J38" s="24" t="n"/>
-      <c r="K38" s="24" t="n"/>
-      <c r="L38" s="24" t="n"/>
-      <c r="M38" s="27" t="n"/>
+      <c r="D38" s="24" t="inlineStr"/>
+      <c r="E38" s="24" t="inlineStr"/>
+      <c r="F38" s="24" t="inlineStr"/>
+      <c r="G38" s="24" t="inlineStr"/>
+      <c r="H38" s="24" t="inlineStr"/>
+      <c r="I38" s="24" t="inlineStr"/>
+      <c r="J38" s="24" t="inlineStr"/>
+      <c r="K38" s="24" t="inlineStr"/>
+      <c r="L38" s="24" t="inlineStr"/>
+      <c r="M38" s="27" t="inlineStr"/>
       <c r="N38" s="1" t="n"/>
       <c r="O38" s="1" t="n"/>
       <c r="P38" s="1" t="n"/>
@@ -2487,16 +2447,16 @@
           <t>1905</t>
         </is>
       </c>
-      <c r="D39" s="24" t="n"/>
-      <c r="E39" s="24" t="n"/>
-      <c r="F39" s="24" t="n"/>
-      <c r="G39" s="24" t="n"/>
-      <c r="H39" s="24" t="n"/>
-      <c r="I39" s="24" t="n"/>
-      <c r="J39" s="24" t="n"/>
-      <c r="K39" s="24" t="n"/>
-      <c r="L39" s="24" t="n"/>
-      <c r="M39" s="27" t="n"/>
+      <c r="D39" s="24" t="inlineStr"/>
+      <c r="E39" s="24" t="inlineStr"/>
+      <c r="F39" s="24" t="inlineStr"/>
+      <c r="G39" s="24" t="inlineStr"/>
+      <c r="H39" s="24" t="inlineStr"/>
+      <c r="I39" s="24" t="inlineStr"/>
+      <c r="J39" s="24" t="inlineStr"/>
+      <c r="K39" s="24" t="inlineStr"/>
+      <c r="L39" s="24" t="inlineStr"/>
+      <c r="M39" s="27" t="inlineStr"/>
       <c r="N39" s="1" t="n"/>
       <c r="O39" s="1" t="n"/>
       <c r="P39" s="1" t="n"/>
@@ -2532,16 +2492,16 @@
           <t>1906</t>
         </is>
       </c>
-      <c r="D40" s="24" t="n"/>
-      <c r="E40" s="24" t="n"/>
-      <c r="F40" s="24" t="n"/>
-      <c r="G40" s="24" t="n"/>
-      <c r="H40" s="24" t="n"/>
-      <c r="I40" s="24" t="n"/>
-      <c r="J40" s="24" t="n"/>
-      <c r="K40" s="24" t="n"/>
-      <c r="L40" s="24" t="n"/>
-      <c r="M40" s="27" t="n"/>
+      <c r="D40" s="24" t="inlineStr"/>
+      <c r="E40" s="24" t="inlineStr"/>
+      <c r="F40" s="24" t="inlineStr"/>
+      <c r="G40" s="24" t="inlineStr"/>
+      <c r="H40" s="24" t="inlineStr"/>
+      <c r="I40" s="24" t="inlineStr"/>
+      <c r="J40" s="24" t="inlineStr"/>
+      <c r="K40" s="24" t="inlineStr"/>
+      <c r="L40" s="24" t="inlineStr"/>
+      <c r="M40" s="27" t="inlineStr"/>
       <c r="N40" s="1" t="n"/>
       <c r="O40" s="1" t="n"/>
       <c r="P40" s="1" t="n"/>
@@ -2577,16 +2537,16 @@
           <t>1907</t>
         </is>
       </c>
-      <c r="D41" s="24" t="n"/>
-      <c r="E41" s="24" t="n"/>
-      <c r="F41" s="24" t="n"/>
-      <c r="G41" s="24" t="n"/>
-      <c r="H41" s="24" t="n"/>
-      <c r="I41" s="24" t="n"/>
-      <c r="J41" s="24" t="n"/>
-      <c r="K41" s="24" t="n"/>
-      <c r="L41" s="24" t="n"/>
-      <c r="M41" s="27" t="n"/>
+      <c r="D41" s="24" t="inlineStr"/>
+      <c r="E41" s="24" t="inlineStr"/>
+      <c r="F41" s="24" t="inlineStr"/>
+      <c r="G41" s="24" t="inlineStr"/>
+      <c r="H41" s="24" t="inlineStr"/>
+      <c r="I41" s="24" t="inlineStr"/>
+      <c r="J41" s="24" t="inlineStr"/>
+      <c r="K41" s="24" t="inlineStr"/>
+      <c r="L41" s="24" t="inlineStr"/>
+      <c r="M41" s="27" t="inlineStr"/>
       <c r="N41" s="1" t="n"/>
       <c r="O41" s="1" t="n"/>
       <c r="P41" s="1" t="n"/>
@@ -2622,16 +2582,16 @@
           <t>1908</t>
         </is>
       </c>
-      <c r="D42" s="24" t="n"/>
-      <c r="E42" s="24" t="n"/>
-      <c r="F42" s="24" t="n"/>
-      <c r="G42" s="24" t="n"/>
-      <c r="H42" s="24" t="n"/>
-      <c r="I42" s="24" t="n"/>
-      <c r="J42" s="24" t="n"/>
-      <c r="K42" s="24" t="n"/>
-      <c r="L42" s="24" t="n"/>
-      <c r="M42" s="27" t="n"/>
+      <c r="D42" s="24" t="inlineStr"/>
+      <c r="E42" s="24" t="inlineStr"/>
+      <c r="F42" s="24" t="inlineStr"/>
+      <c r="G42" s="24" t="inlineStr"/>
+      <c r="H42" s="24" t="inlineStr"/>
+      <c r="I42" s="24" t="inlineStr"/>
+      <c r="J42" s="24" t="inlineStr"/>
+      <c r="K42" s="24" t="inlineStr"/>
+      <c r="L42" s="24" t="inlineStr"/>
+      <c r="M42" s="27" t="inlineStr"/>
       <c r="N42" s="1" t="n"/>
       <c r="O42" s="1" t="n"/>
       <c r="P42" s="1" t="n"/>
@@ -2667,16 +2627,16 @@
           <t>1909</t>
         </is>
       </c>
-      <c r="D43" s="24" t="n"/>
-      <c r="E43" s="24" t="n"/>
-      <c r="F43" s="24" t="n"/>
-      <c r="G43" s="24" t="n"/>
-      <c r="H43" s="24" t="n"/>
-      <c r="I43" s="24" t="n"/>
-      <c r="J43" s="24" t="n"/>
-      <c r="K43" s="24" t="n"/>
-      <c r="L43" s="24" t="n"/>
-      <c r="M43" s="27" t="n"/>
+      <c r="D43" s="24" t="inlineStr"/>
+      <c r="E43" s="24" t="inlineStr"/>
+      <c r="F43" s="24" t="inlineStr"/>
+      <c r="G43" s="24" t="inlineStr"/>
+      <c r="H43" s="24" t="inlineStr"/>
+      <c r="I43" s="24" t="inlineStr"/>
+      <c r="J43" s="24" t="inlineStr"/>
+      <c r="K43" s="24" t="inlineStr"/>
+      <c r="L43" s="24" t="inlineStr"/>
+      <c r="M43" s="27" t="inlineStr"/>
       <c r="N43" s="1" t="n"/>
       <c r="O43" s="1" t="n"/>
       <c r="P43" s="1" t="n"/>
@@ -2712,16 +2672,16 @@
           <t>1910</t>
         </is>
       </c>
-      <c r="D44" s="24" t="n"/>
-      <c r="E44" s="24" t="n"/>
-      <c r="F44" s="24" t="n"/>
-      <c r="G44" s="24" t="n"/>
-      <c r="H44" s="24" t="n"/>
-      <c r="I44" s="24" t="n"/>
-      <c r="J44" s="24" t="n"/>
-      <c r="K44" s="24" t="n"/>
-      <c r="L44" s="24" t="n"/>
-      <c r="M44" s="27" t="n"/>
+      <c r="D44" s="24" t="inlineStr"/>
+      <c r="E44" s="24" t="inlineStr"/>
+      <c r="F44" s="24" t="inlineStr"/>
+      <c r="G44" s="24" t="inlineStr"/>
+      <c r="H44" s="24" t="inlineStr"/>
+      <c r="I44" s="24" t="inlineStr"/>
+      <c r="J44" s="24" t="inlineStr"/>
+      <c r="K44" s="24" t="inlineStr"/>
+      <c r="L44" s="24" t="inlineStr"/>
+      <c r="M44" s="27" t="inlineStr"/>
       <c r="N44" s="1" t="n"/>
       <c r="O44" s="1" t="n"/>
       <c r="P44" s="1" t="n"/>
@@ -2757,16 +2717,16 @@
           <t>1909–1910</t>
         </is>
       </c>
-      <c r="D45" s="24" t="n"/>
-      <c r="E45" s="24" t="n"/>
-      <c r="F45" s="24" t="n"/>
-      <c r="G45" s="24" t="n"/>
-      <c r="H45" s="24" t="n"/>
-      <c r="I45" s="24" t="n"/>
-      <c r="J45" s="24" t="n"/>
-      <c r="K45" s="24" t="n"/>
-      <c r="L45" s="24" t="n"/>
-      <c r="M45" s="27" t="n"/>
+      <c r="D45" s="24" t="inlineStr"/>
+      <c r="E45" s="24" t="inlineStr"/>
+      <c r="F45" s="24" t="inlineStr"/>
+      <c r="G45" s="24" t="inlineStr"/>
+      <c r="H45" s="24" t="inlineStr"/>
+      <c r="I45" s="24" t="inlineStr"/>
+      <c r="J45" s="24" t="inlineStr"/>
+      <c r="K45" s="24" t="inlineStr"/>
+      <c r="L45" s="24" t="inlineStr"/>
+      <c r="M45" s="27" t="inlineStr"/>
       <c r="N45" s="1" t="n"/>
       <c r="O45" s="1" t="n"/>
       <c r="P45" s="1" t="n"/>
@@ -2802,16 +2762,16 @@
           <t>1910</t>
         </is>
       </c>
-      <c r="D46" s="24" t="n"/>
-      <c r="E46" s="24" t="n"/>
-      <c r="F46" s="24" t="n"/>
-      <c r="G46" s="24" t="n"/>
-      <c r="H46" s="24" t="n"/>
-      <c r="I46" s="24" t="n"/>
-      <c r="J46" s="24" t="n"/>
-      <c r="K46" s="24" t="n"/>
-      <c r="L46" s="24" t="n"/>
-      <c r="M46" s="27" t="n"/>
+      <c r="D46" s="24" t="inlineStr"/>
+      <c r="E46" s="24" t="inlineStr"/>
+      <c r="F46" s="24" t="inlineStr"/>
+      <c r="G46" s="24" t="inlineStr"/>
+      <c r="H46" s="24" t="inlineStr"/>
+      <c r="I46" s="24" t="inlineStr"/>
+      <c r="J46" s="24" t="inlineStr"/>
+      <c r="K46" s="24" t="inlineStr"/>
+      <c r="L46" s="24" t="inlineStr"/>
+      <c r="M46" s="27" t="inlineStr"/>
       <c r="N46" s="1" t="n"/>
       <c r="O46" s="1" t="n"/>
       <c r="P46" s="1" t="n"/>
@@ -2847,16 +2807,16 @@
           <t>1911</t>
         </is>
       </c>
-      <c r="D47" s="24" t="n"/>
-      <c r="E47" s="24" t="n"/>
-      <c r="F47" s="24" t="n"/>
-      <c r="G47" s="24" t="n"/>
-      <c r="H47" s="24" t="n"/>
-      <c r="I47" s="24" t="n"/>
-      <c r="J47" s="24" t="n"/>
-      <c r="K47" s="24" t="n"/>
-      <c r="L47" s="24" t="n"/>
-      <c r="M47" s="27" t="n"/>
+      <c r="D47" s="24" t="inlineStr"/>
+      <c r="E47" s="24" t="inlineStr"/>
+      <c r="F47" s="24" t="inlineStr"/>
+      <c r="G47" s="24" t="inlineStr"/>
+      <c r="H47" s="24" t="inlineStr"/>
+      <c r="I47" s="24" t="inlineStr"/>
+      <c r="J47" s="24" t="inlineStr"/>
+      <c r="K47" s="24" t="inlineStr"/>
+      <c r="L47" s="24" t="inlineStr"/>
+      <c r="M47" s="27" t="inlineStr"/>
       <c r="N47" s="1" t="n"/>
       <c r="O47" s="1" t="n"/>
       <c r="P47" s="1" t="n"/>
@@ -2892,16 +2852,16 @@
           <t>1912</t>
         </is>
       </c>
-      <c r="D48" s="24" t="n"/>
-      <c r="E48" s="24" t="n"/>
-      <c r="F48" s="24" t="n"/>
-      <c r="G48" s="24" t="n"/>
-      <c r="H48" s="24" t="n"/>
-      <c r="I48" s="24" t="n"/>
-      <c r="J48" s="24" t="n"/>
-      <c r="K48" s="24" t="n"/>
-      <c r="L48" s="24" t="n"/>
-      <c r="M48" s="27" t="n"/>
+      <c r="D48" s="24" t="inlineStr"/>
+      <c r="E48" s="24" t="inlineStr"/>
+      <c r="F48" s="24" t="inlineStr"/>
+      <c r="G48" s="24" t="inlineStr"/>
+      <c r="H48" s="24" t="inlineStr"/>
+      <c r="I48" s="24" t="inlineStr"/>
+      <c r="J48" s="24" t="inlineStr"/>
+      <c r="K48" s="24" t="inlineStr"/>
+      <c r="L48" s="24" t="inlineStr"/>
+      <c r="M48" s="27" t="inlineStr"/>
       <c r="N48" s="1" t="n"/>
       <c r="O48" s="1" t="n"/>
       <c r="P48" s="1" t="n"/>
@@ -2937,16 +2897,16 @@
           <t>1913</t>
         </is>
       </c>
-      <c r="D49" s="24" t="n"/>
-      <c r="E49" s="24" t="n"/>
-      <c r="F49" s="24" t="n"/>
-      <c r="G49" s="24" t="n"/>
-      <c r="H49" s="24" t="n"/>
-      <c r="I49" s="24" t="n"/>
-      <c r="J49" s="24" t="n"/>
-      <c r="K49" s="24" t="n"/>
-      <c r="L49" s="24" t="n"/>
-      <c r="M49" s="27" t="n"/>
+      <c r="D49" s="24" t="inlineStr"/>
+      <c r="E49" s="24" t="inlineStr"/>
+      <c r="F49" s="24" t="inlineStr"/>
+      <c r="G49" s="24" t="inlineStr"/>
+      <c r="H49" s="24" t="inlineStr"/>
+      <c r="I49" s="24" t="inlineStr"/>
+      <c r="J49" s="24" t="inlineStr"/>
+      <c r="K49" s="24" t="inlineStr"/>
+      <c r="L49" s="24" t="inlineStr"/>
+      <c r="M49" s="27" t="inlineStr"/>
       <c r="N49" s="1" t="n"/>
       <c r="O49" s="1" t="n"/>
       <c r="P49" s="1" t="n"/>
@@ -2982,16 +2942,16 @@
           <t>1914</t>
         </is>
       </c>
-      <c r="D50" s="24" t="n"/>
-      <c r="E50" s="24" t="n"/>
-      <c r="F50" s="24" t="n"/>
-      <c r="G50" s="24" t="n"/>
-      <c r="H50" s="24" t="n"/>
-      <c r="I50" s="24" t="n"/>
-      <c r="J50" s="24" t="n"/>
-      <c r="K50" s="24" t="n"/>
-      <c r="L50" s="24" t="n"/>
-      <c r="M50" s="27" t="n"/>
+      <c r="D50" s="24" t="inlineStr"/>
+      <c r="E50" s="24" t="inlineStr"/>
+      <c r="F50" s="24" t="inlineStr"/>
+      <c r="G50" s="24" t="inlineStr"/>
+      <c r="H50" s="24" t="inlineStr"/>
+      <c r="I50" s="24" t="inlineStr"/>
+      <c r="J50" s="24" t="inlineStr"/>
+      <c r="K50" s="24" t="inlineStr"/>
+      <c r="L50" s="24" t="inlineStr"/>
+      <c r="M50" s="27" t="inlineStr"/>
       <c r="N50" s="1" t="n"/>
       <c r="O50" s="1" t="n"/>
       <c r="P50" s="1" t="n"/>
@@ -3027,16 +2987,16 @@
           <t>1915</t>
         </is>
       </c>
-      <c r="D51" s="24" t="n"/>
-      <c r="E51" s="24" t="n"/>
-      <c r="F51" s="24" t="n"/>
-      <c r="G51" s="24" t="n"/>
-      <c r="H51" s="24" t="n"/>
-      <c r="I51" s="24" t="n"/>
-      <c r="J51" s="24" t="n"/>
-      <c r="K51" s="24" t="n"/>
-      <c r="L51" s="24" t="n"/>
-      <c r="M51" s="27" t="n"/>
+      <c r="D51" s="24" t="inlineStr"/>
+      <c r="E51" s="24" t="inlineStr"/>
+      <c r="F51" s="24" t="inlineStr"/>
+      <c r="G51" s="24" t="inlineStr"/>
+      <c r="H51" s="24" t="inlineStr"/>
+      <c r="I51" s="24" t="inlineStr"/>
+      <c r="J51" s="24" t="inlineStr"/>
+      <c r="K51" s="24" t="inlineStr"/>
+      <c r="L51" s="24" t="inlineStr"/>
+      <c r="M51" s="27" t="inlineStr"/>
       <c r="N51" s="1" t="n"/>
       <c r="O51" s="1" t="n"/>
       <c r="P51" s="1" t="n"/>
@@ -3072,16 +3032,16 @@
           <t>1916</t>
         </is>
       </c>
-      <c r="D52" s="24" t="n"/>
-      <c r="E52" s="24" t="n"/>
-      <c r="F52" s="24" t="n"/>
-      <c r="G52" s="24" t="n"/>
-      <c r="H52" s="24" t="n"/>
-      <c r="I52" s="24" t="n"/>
-      <c r="J52" s="24" t="n"/>
-      <c r="K52" s="24" t="n"/>
-      <c r="L52" s="24" t="n"/>
-      <c r="M52" s="27" t="n"/>
+      <c r="D52" s="24" t="inlineStr"/>
+      <c r="E52" s="24" t="inlineStr"/>
+      <c r="F52" s="24" t="inlineStr"/>
+      <c r="G52" s="24" t="inlineStr"/>
+      <c r="H52" s="24" t="inlineStr"/>
+      <c r="I52" s="24" t="inlineStr"/>
+      <c r="J52" s="24" t="inlineStr"/>
+      <c r="K52" s="24" t="inlineStr"/>
+      <c r="L52" s="24" t="inlineStr"/>
+      <c r="M52" s="27" t="inlineStr"/>
       <c r="N52" s="1" t="n"/>
       <c r="O52" s="1" t="n"/>
       <c r="P52" s="1" t="n"/>
@@ -3117,16 +3077,16 @@
           <t>1917</t>
         </is>
       </c>
-      <c r="D53" s="24" t="n"/>
-      <c r="E53" s="24" t="n"/>
-      <c r="F53" s="24" t="n"/>
-      <c r="G53" s="24" t="n"/>
-      <c r="H53" s="24" t="n"/>
-      <c r="I53" s="24" t="n"/>
-      <c r="J53" s="24" t="n"/>
-      <c r="K53" s="24" t="n"/>
-      <c r="L53" s="24" t="n"/>
-      <c r="M53" s="27" t="n"/>
+      <c r="D53" s="24" t="inlineStr"/>
+      <c r="E53" s="24" t="inlineStr"/>
+      <c r="F53" s="24" t="inlineStr"/>
+      <c r="G53" s="24" t="inlineStr"/>
+      <c r="H53" s="24" t="inlineStr"/>
+      <c r="I53" s="24" t="inlineStr"/>
+      <c r="J53" s="24" t="inlineStr"/>
+      <c r="K53" s="24" t="inlineStr"/>
+      <c r="L53" s="24" t="inlineStr"/>
+      <c r="M53" s="27" t="inlineStr"/>
       <c r="N53" s="1" t="n"/>
       <c r="O53" s="1" t="n"/>
       <c r="P53" s="1" t="n"/>
@@ -3162,16 +3122,16 @@
           <t>1918</t>
         </is>
       </c>
-      <c r="D54" s="24" t="n"/>
-      <c r="E54" s="24" t="n"/>
-      <c r="F54" s="24" t="n"/>
-      <c r="G54" s="24" t="n"/>
-      <c r="H54" s="24" t="n"/>
-      <c r="I54" s="24" t="n"/>
-      <c r="J54" s="24" t="n"/>
-      <c r="K54" s="24" t="n"/>
-      <c r="L54" s="24" t="n"/>
-      <c r="M54" s="27" t="n"/>
+      <c r="D54" s="24" t="inlineStr"/>
+      <c r="E54" s="24" t="inlineStr"/>
+      <c r="F54" s="24" t="inlineStr"/>
+      <c r="G54" s="24" t="inlineStr"/>
+      <c r="H54" s="24" t="inlineStr"/>
+      <c r="I54" s="24" t="inlineStr"/>
+      <c r="J54" s="24" t="inlineStr"/>
+      <c r="K54" s="24" t="inlineStr"/>
+      <c r="L54" s="24" t="inlineStr"/>
+      <c r="M54" s="27" t="inlineStr"/>
       <c r="N54" s="1" t="n"/>
       <c r="O54" s="1" t="n"/>
       <c r="P54" s="1" t="n"/>
@@ -3207,16 +3167,16 @@
           <t>1919</t>
         </is>
       </c>
-      <c r="D55" s="24" t="n"/>
-      <c r="E55" s="24" t="n"/>
-      <c r="F55" s="24" t="n"/>
-      <c r="G55" s="24" t="n"/>
-      <c r="H55" s="24" t="n"/>
-      <c r="I55" s="24" t="n"/>
-      <c r="J55" s="24" t="n"/>
-      <c r="K55" s="24" t="n"/>
-      <c r="L55" s="24" t="n"/>
-      <c r="M55" s="27" t="n"/>
+      <c r="D55" s="24" t="inlineStr"/>
+      <c r="E55" s="24" t="inlineStr"/>
+      <c r="F55" s="24" t="inlineStr"/>
+      <c r="G55" s="24" t="inlineStr"/>
+      <c r="H55" s="24" t="inlineStr"/>
+      <c r="I55" s="24" t="inlineStr"/>
+      <c r="J55" s="24" t="inlineStr"/>
+      <c r="K55" s="24" t="inlineStr"/>
+      <c r="L55" s="24" t="inlineStr"/>
+      <c r="M55" s="27" t="inlineStr"/>
       <c r="N55" s="1" t="n"/>
       <c r="O55" s="1" t="n"/>
       <c r="P55" s="1" t="n"/>
@@ -3252,16 +3212,16 @@
           <t>1797–1914</t>
         </is>
       </c>
-      <c r="D56" s="24" t="n"/>
-      <c r="E56" s="24" t="n"/>
-      <c r="F56" s="24" t="n"/>
-      <c r="G56" s="24" t="n"/>
-      <c r="H56" s="24" t="n"/>
-      <c r="I56" s="24" t="n"/>
-      <c r="J56" s="24" t="n"/>
-      <c r="K56" s="24" t="n"/>
-      <c r="L56" s="24" t="n"/>
-      <c r="M56" s="27" t="n"/>
+      <c r="D56" s="24" t="inlineStr"/>
+      <c r="E56" s="24" t="inlineStr"/>
+      <c r="F56" s="24" t="inlineStr"/>
+      <c r="G56" s="24" t="inlineStr"/>
+      <c r="H56" s="24" t="inlineStr"/>
+      <c r="I56" s="24" t="inlineStr"/>
+      <c r="J56" s="24" t="inlineStr"/>
+      <c r="K56" s="24" t="inlineStr"/>
+      <c r="L56" s="24" t="inlineStr"/>
+      <c r="M56" s="27" t="inlineStr"/>
       <c r="N56" s="1" t="n"/>
       <c r="O56" s="1" t="n"/>
       <c r="P56" s="1" t="n"/>
@@ -3297,16 +3257,16 @@
           <t>1909</t>
         </is>
       </c>
-      <c r="D57" s="24" t="n"/>
-      <c r="E57" s="24" t="n"/>
-      <c r="F57" s="24" t="n"/>
-      <c r="G57" s="24" t="n"/>
-      <c r="H57" s="24" t="n"/>
-      <c r="I57" s="24" t="n"/>
-      <c r="J57" s="24" t="n"/>
-      <c r="K57" s="24" t="n"/>
-      <c r="L57" s="24" t="n"/>
-      <c r="M57" s="27" t="n"/>
+      <c r="D57" s="24" t="inlineStr"/>
+      <c r="E57" s="24" t="inlineStr"/>
+      <c r="F57" s="24" t="inlineStr"/>
+      <c r="G57" s="24" t="inlineStr"/>
+      <c r="H57" s="24" t="inlineStr"/>
+      <c r="I57" s="24" t="inlineStr"/>
+      <c r="J57" s="24" t="inlineStr"/>
+      <c r="K57" s="24" t="inlineStr"/>
+      <c r="L57" s="24" t="inlineStr"/>
+      <c r="M57" s="27" t="inlineStr"/>
       <c r="N57" s="1" t="n"/>
       <c r="O57" s="1" t="n"/>
       <c r="P57" s="1" t="n"/>
@@ -3342,16 +3302,16 @@
           <t>1913–1915</t>
         </is>
       </c>
-      <c r="D58" s="24" t="n"/>
-      <c r="E58" s="24" t="n"/>
-      <c r="F58" s="24" t="n"/>
-      <c r="G58" s="24" t="n"/>
-      <c r="H58" s="24" t="n"/>
-      <c r="I58" s="24" t="n"/>
-      <c r="J58" s="24" t="n"/>
-      <c r="K58" s="24" t="n"/>
-      <c r="L58" s="24" t="n"/>
-      <c r="M58" s="27" t="n"/>
+      <c r="D58" s="24" t="inlineStr"/>
+      <c r="E58" s="24" t="inlineStr"/>
+      <c r="F58" s="24" t="inlineStr"/>
+      <c r="G58" s="24" t="inlineStr"/>
+      <c r="H58" s="24" t="inlineStr"/>
+      <c r="I58" s="24" t="inlineStr"/>
+      <c r="J58" s="24" t="inlineStr"/>
+      <c r="K58" s="24" t="inlineStr"/>
+      <c r="L58" s="24" t="inlineStr"/>
+      <c r="M58" s="27" t="inlineStr"/>
       <c r="N58" s="1" t="n"/>
       <c r="O58" s="1" t="n"/>
       <c r="P58" s="1" t="n"/>
@@ -3387,16 +3347,16 @@
           <t>1917</t>
         </is>
       </c>
-      <c r="D59" s="24" t="n"/>
-      <c r="E59" s="24" t="n"/>
-      <c r="F59" s="24" t="n"/>
-      <c r="G59" s="24" t="n"/>
-      <c r="H59" s="24" t="n"/>
-      <c r="I59" s="24" t="n"/>
-      <c r="J59" s="24" t="n"/>
-      <c r="K59" s="24" t="n"/>
-      <c r="L59" s="24" t="n"/>
-      <c r="M59" s="27" t="n"/>
+      <c r="D59" s="24" t="inlineStr"/>
+      <c r="E59" s="24" t="inlineStr"/>
+      <c r="F59" s="24" t="inlineStr"/>
+      <c r="G59" s="24" t="inlineStr"/>
+      <c r="H59" s="24" t="inlineStr"/>
+      <c r="I59" s="24" t="inlineStr"/>
+      <c r="J59" s="24" t="inlineStr"/>
+      <c r="K59" s="24" t="inlineStr"/>
+      <c r="L59" s="24" t="inlineStr"/>
+      <c r="M59" s="27" t="inlineStr"/>
       <c r="N59" s="1" t="n"/>
       <c r="O59" s="1" t="n"/>
       <c r="P59" s="1" t="n"/>
@@ -3432,16 +3392,16 @@
           <t>1911</t>
         </is>
       </c>
-      <c r="D60" s="24" t="n"/>
-      <c r="E60" s="24" t="n"/>
-      <c r="F60" s="24" t="n"/>
-      <c r="G60" s="24" t="n"/>
-      <c r="H60" s="24" t="n"/>
-      <c r="I60" s="24" t="n"/>
-      <c r="J60" s="24" t="n"/>
-      <c r="K60" s="24" t="n"/>
-      <c r="L60" s="24" t="n"/>
-      <c r="M60" s="27" t="n"/>
+      <c r="D60" s="24" t="inlineStr"/>
+      <c r="E60" s="24" t="inlineStr"/>
+      <c r="F60" s="24" t="inlineStr"/>
+      <c r="G60" s="24" t="inlineStr"/>
+      <c r="H60" s="24" t="inlineStr"/>
+      <c r="I60" s="24" t="inlineStr"/>
+      <c r="J60" s="24" t="inlineStr"/>
+      <c r="K60" s="24" t="inlineStr"/>
+      <c r="L60" s="24" t="inlineStr"/>
+      <c r="M60" s="27" t="inlineStr"/>
       <c r="N60" s="1" t="n"/>
       <c r="O60" s="1" t="n"/>
       <c r="P60" s="1" t="n"/>
@@ -3477,16 +3437,16 @@
           <t>1912</t>
         </is>
       </c>
-      <c r="D61" s="24" t="n"/>
-      <c r="E61" s="24" t="n"/>
-      <c r="F61" s="24" t="n"/>
-      <c r="G61" s="24" t="n"/>
-      <c r="H61" s="24" t="n"/>
-      <c r="I61" s="24" t="n"/>
-      <c r="J61" s="24" t="n"/>
-      <c r="K61" s="24" t="n"/>
-      <c r="L61" s="24" t="n"/>
-      <c r="M61" s="27" t="n"/>
+      <c r="D61" s="24" t="inlineStr"/>
+      <c r="E61" s="24" t="inlineStr"/>
+      <c r="F61" s="24" t="inlineStr"/>
+      <c r="G61" s="24" t="inlineStr"/>
+      <c r="H61" s="24" t="inlineStr"/>
+      <c r="I61" s="24" t="inlineStr"/>
+      <c r="J61" s="24" t="inlineStr"/>
+      <c r="K61" s="24" t="inlineStr"/>
+      <c r="L61" s="24" t="inlineStr"/>
+      <c r="M61" s="27" t="inlineStr"/>
       <c r="N61" s="1" t="n"/>
       <c r="O61" s="1" t="n"/>
       <c r="P61" s="1" t="n"/>
@@ -3522,16 +3482,16 @@
           <t>1913</t>
         </is>
       </c>
-      <c r="D62" s="24" t="n"/>
-      <c r="E62" s="24" t="n"/>
-      <c r="F62" s="24" t="n"/>
-      <c r="G62" s="24" t="n"/>
-      <c r="H62" s="24" t="n"/>
-      <c r="I62" s="24" t="n"/>
-      <c r="J62" s="24" t="n"/>
-      <c r="K62" s="24" t="n"/>
-      <c r="L62" s="24" t="n"/>
-      <c r="M62" s="27" t="n"/>
+      <c r="D62" s="24" t="inlineStr"/>
+      <c r="E62" s="24" t="inlineStr"/>
+      <c r="F62" s="24" t="inlineStr"/>
+      <c r="G62" s="24" t="inlineStr"/>
+      <c r="H62" s="24" t="inlineStr"/>
+      <c r="I62" s="24" t="inlineStr"/>
+      <c r="J62" s="24" t="inlineStr"/>
+      <c r="K62" s="24" t="inlineStr"/>
+      <c r="L62" s="24" t="inlineStr"/>
+      <c r="M62" s="27" t="inlineStr"/>
       <c r="N62" s="1" t="n"/>
       <c r="O62" s="1" t="n"/>
       <c r="P62" s="1" t="n"/>
@@ -3567,16 +3527,16 @@
           <t>1914</t>
         </is>
       </c>
-      <c r="D63" s="24" t="n"/>
-      <c r="E63" s="24" t="n"/>
-      <c r="F63" s="24" t="n"/>
-      <c r="G63" s="24" t="n"/>
-      <c r="H63" s="24" t="n"/>
-      <c r="I63" s="24" t="n"/>
-      <c r="J63" s="24" t="n"/>
-      <c r="K63" s="24" t="n"/>
-      <c r="L63" s="24" t="n"/>
-      <c r="M63" s="27" t="n"/>
+      <c r="D63" s="24" t="inlineStr"/>
+      <c r="E63" s="24" t="inlineStr"/>
+      <c r="F63" s="24" t="inlineStr"/>
+      <c r="G63" s="24" t="inlineStr"/>
+      <c r="H63" s="24" t="inlineStr"/>
+      <c r="I63" s="24" t="inlineStr"/>
+      <c r="J63" s="24" t="inlineStr"/>
+      <c r="K63" s="24" t="inlineStr"/>
+      <c r="L63" s="24" t="inlineStr"/>
+      <c r="M63" s="27" t="inlineStr"/>
       <c r="N63" s="1" t="n"/>
       <c r="O63" s="1" t="n"/>
       <c r="P63" s="1" t="n"/>
@@ -3612,16 +3572,16 @@
           <t>1915</t>
         </is>
       </c>
-      <c r="D64" s="24" t="n"/>
-      <c r="E64" s="24" t="n"/>
-      <c r="F64" s="24" t="n"/>
-      <c r="G64" s="24" t="n"/>
-      <c r="H64" s="24" t="n"/>
-      <c r="I64" s="24" t="n"/>
-      <c r="J64" s="24" t="n"/>
-      <c r="K64" s="24" t="n"/>
-      <c r="L64" s="24" t="n"/>
-      <c r="M64" s="27" t="n"/>
+      <c r="D64" s="24" t="inlineStr"/>
+      <c r="E64" s="24" t="inlineStr"/>
+      <c r="F64" s="24" t="inlineStr"/>
+      <c r="G64" s="24" t="inlineStr"/>
+      <c r="H64" s="24" t="inlineStr"/>
+      <c r="I64" s="24" t="inlineStr"/>
+      <c r="J64" s="24" t="inlineStr"/>
+      <c r="K64" s="24" t="inlineStr"/>
+      <c r="L64" s="24" t="inlineStr"/>
+      <c r="M64" s="27" t="inlineStr"/>
       <c r="N64" s="1" t="n"/>
       <c r="O64" s="1" t="n"/>
       <c r="P64" s="1" t="n"/>
@@ -3657,16 +3617,16 @@
           <t>1916</t>
         </is>
       </c>
-      <c r="D65" s="24" t="n"/>
-      <c r="E65" s="24" t="n"/>
-      <c r="F65" s="24" t="n"/>
-      <c r="G65" s="24" t="n"/>
-      <c r="H65" s="24" t="n"/>
-      <c r="I65" s="24" t="n"/>
-      <c r="J65" s="24" t="n"/>
-      <c r="K65" s="24" t="n"/>
-      <c r="L65" s="24" t="n"/>
-      <c r="M65" s="27" t="n"/>
+      <c r="D65" s="24" t="inlineStr"/>
+      <c r="E65" s="24" t="inlineStr"/>
+      <c r="F65" s="24" t="inlineStr"/>
+      <c r="G65" s="24" t="inlineStr"/>
+      <c r="H65" s="24" t="inlineStr"/>
+      <c r="I65" s="24" t="inlineStr"/>
+      <c r="J65" s="24" t="inlineStr"/>
+      <c r="K65" s="24" t="inlineStr"/>
+      <c r="L65" s="24" t="inlineStr"/>
+      <c r="M65" s="27" t="inlineStr"/>
       <c r="N65" s="1" t="n"/>
       <c r="O65" s="1" t="n"/>
       <c r="P65" s="1" t="n"/>
@@ -3702,16 +3662,16 @@
           <t>1917</t>
         </is>
       </c>
-      <c r="D66" s="24" t="n"/>
-      <c r="E66" s="24" t="n"/>
-      <c r="F66" s="24" t="n"/>
-      <c r="G66" s="24" t="n"/>
-      <c r="H66" s="24" t="n"/>
-      <c r="I66" s="24" t="n"/>
-      <c r="J66" s="24" t="n"/>
-      <c r="K66" s="24" t="n"/>
-      <c r="L66" s="24" t="n"/>
-      <c r="M66" s="27" t="n"/>
+      <c r="D66" s="24" t="inlineStr"/>
+      <c r="E66" s="24" t="inlineStr"/>
+      <c r="F66" s="24" t="inlineStr"/>
+      <c r="G66" s="24" t="inlineStr"/>
+      <c r="H66" s="24" t="inlineStr"/>
+      <c r="I66" s="24" t="inlineStr"/>
+      <c r="J66" s="24" t="inlineStr"/>
+      <c r="K66" s="24" t="inlineStr"/>
+      <c r="L66" s="24" t="inlineStr"/>
+      <c r="M66" s="27" t="inlineStr"/>
       <c r="N66" s="1" t="n"/>
       <c r="O66" s="1" t="n"/>
       <c r="P66" s="1" t="n"/>
@@ -3747,16 +3707,16 @@
           <t>1918</t>
         </is>
       </c>
-      <c r="D67" s="24" t="n"/>
-      <c r="E67" s="24" t="n"/>
-      <c r="F67" s="24" t="n"/>
-      <c r="G67" s="24" t="n"/>
-      <c r="H67" s="24" t="n"/>
-      <c r="I67" s="24" t="n"/>
-      <c r="J67" s="24" t="n"/>
-      <c r="K67" s="24" t="n"/>
-      <c r="L67" s="24" t="n"/>
-      <c r="M67" s="27" t="n"/>
+      <c r="D67" s="24" t="inlineStr"/>
+      <c r="E67" s="24" t="inlineStr"/>
+      <c r="F67" s="24" t="inlineStr"/>
+      <c r="G67" s="24" t="inlineStr"/>
+      <c r="H67" s="24" t="inlineStr"/>
+      <c r="I67" s="24" t="inlineStr"/>
+      <c r="J67" s="24" t="inlineStr"/>
+      <c r="K67" s="24" t="inlineStr"/>
+      <c r="L67" s="24" t="inlineStr"/>
+      <c r="M67" s="27" t="inlineStr"/>
       <c r="N67" s="1" t="n"/>
       <c r="O67" s="1" t="n"/>
       <c r="P67" s="1" t="n"/>
@@ -3792,16 +3752,16 @@
           <t>1919</t>
         </is>
       </c>
-      <c r="D68" s="24" t="n"/>
-      <c r="E68" s="24" t="n"/>
-      <c r="F68" s="24" t="n"/>
-      <c r="G68" s="24" t="n"/>
-      <c r="H68" s="24" t="n"/>
-      <c r="I68" s="24" t="n"/>
-      <c r="J68" s="24" t="n"/>
-      <c r="K68" s="24" t="n"/>
-      <c r="L68" s="24" t="n"/>
-      <c r="M68" s="27" t="n"/>
+      <c r="D68" s="24" t="inlineStr"/>
+      <c r="E68" s="24" t="inlineStr"/>
+      <c r="F68" s="24" t="inlineStr"/>
+      <c r="G68" s="24" t="inlineStr"/>
+      <c r="H68" s="24" t="inlineStr"/>
+      <c r="I68" s="24" t="inlineStr"/>
+      <c r="J68" s="24" t="inlineStr"/>
+      <c r="K68" s="24" t="inlineStr"/>
+      <c r="L68" s="24" t="inlineStr"/>
+      <c r="M68" s="27" t="inlineStr"/>
       <c r="N68" s="1" t="n"/>
       <c r="O68" s="1" t="n"/>
       <c r="P68" s="1" t="n"/>
@@ -3837,16 +3797,16 @@
           <t>1909</t>
         </is>
       </c>
-      <c r="D69" s="24" t="n"/>
-      <c r="E69" s="24" t="n"/>
-      <c r="F69" s="24" t="n"/>
-      <c r="G69" s="24" t="n"/>
-      <c r="H69" s="24" t="n"/>
-      <c r="I69" s="24" t="n"/>
-      <c r="J69" s="24" t="n"/>
-      <c r="K69" s="24" t="n"/>
-      <c r="L69" s="24" t="n"/>
-      <c r="M69" s="27" t="n"/>
+      <c r="D69" s="24" t="inlineStr"/>
+      <c r="E69" s="24" t="inlineStr"/>
+      <c r="F69" s="24" t="inlineStr"/>
+      <c r="G69" s="24" t="inlineStr"/>
+      <c r="H69" s="24" t="inlineStr"/>
+      <c r="I69" s="24" t="inlineStr"/>
+      <c r="J69" s="24" t="inlineStr"/>
+      <c r="K69" s="24" t="inlineStr"/>
+      <c r="L69" s="24" t="inlineStr"/>
+      <c r="M69" s="27" t="inlineStr"/>
       <c r="N69" s="1" t="n"/>
       <c r="O69" s="1" t="n"/>
       <c r="P69" s="1" t="n"/>
@@ -3882,16 +3842,16 @@
           <t>1911</t>
         </is>
       </c>
-      <c r="D70" s="24" t="n"/>
-      <c r="E70" s="24" t="n"/>
-      <c r="F70" s="24" t="n"/>
-      <c r="G70" s="24" t="n"/>
-      <c r="H70" s="24" t="n"/>
-      <c r="I70" s="24" t="n"/>
-      <c r="J70" s="24" t="n"/>
-      <c r="K70" s="24" t="n"/>
-      <c r="L70" s="24" t="n"/>
-      <c r="M70" s="27" t="n"/>
+      <c r="D70" s="24" t="inlineStr"/>
+      <c r="E70" s="24" t="inlineStr"/>
+      <c r="F70" s="24" t="inlineStr"/>
+      <c r="G70" s="24" t="inlineStr"/>
+      <c r="H70" s="24" t="inlineStr"/>
+      <c r="I70" s="24" t="inlineStr"/>
+      <c r="J70" s="24" t="inlineStr"/>
+      <c r="K70" s="24" t="inlineStr"/>
+      <c r="L70" s="24" t="inlineStr"/>
+      <c r="M70" s="27" t="inlineStr"/>
       <c r="N70" s="1" t="n"/>
       <c r="O70" s="1" t="n"/>
       <c r="P70" s="1" t="n"/>
@@ -3927,16 +3887,16 @@
           <t>1912</t>
         </is>
       </c>
-      <c r="D71" s="24" t="n"/>
-      <c r="E71" s="24" t="n"/>
-      <c r="F71" s="24" t="n"/>
-      <c r="G71" s="24" t="n"/>
-      <c r="H71" s="24" t="n"/>
-      <c r="I71" s="24" t="n"/>
-      <c r="J71" s="24" t="n"/>
-      <c r="K71" s="24" t="n"/>
-      <c r="L71" s="24" t="n"/>
-      <c r="M71" s="27" t="n"/>
+      <c r="D71" s="24" t="inlineStr"/>
+      <c r="E71" s="24" t="inlineStr"/>
+      <c r="F71" s="24" t="inlineStr"/>
+      <c r="G71" s="24" t="inlineStr"/>
+      <c r="H71" s="24" t="inlineStr"/>
+      <c r="I71" s="24" t="inlineStr"/>
+      <c r="J71" s="24" t="inlineStr"/>
+      <c r="K71" s="24" t="inlineStr"/>
+      <c r="L71" s="24" t="inlineStr"/>
+      <c r="M71" s="27" t="inlineStr"/>
       <c r="N71" s="1" t="n"/>
       <c r="O71" s="1" t="n"/>
       <c r="P71" s="1" t="n"/>
@@ -3972,16 +3932,16 @@
           <t>1913</t>
         </is>
       </c>
-      <c r="D72" s="24" t="n"/>
-      <c r="E72" s="24" t="n"/>
-      <c r="F72" s="24" t="n"/>
-      <c r="G72" s="24" t="n"/>
-      <c r="H72" s="24" t="n"/>
-      <c r="I72" s="24" t="n"/>
-      <c r="J72" s="24" t="n"/>
-      <c r="K72" s="24" t="n"/>
-      <c r="L72" s="24" t="n"/>
-      <c r="M72" s="27" t="n"/>
+      <c r="D72" s="24" t="inlineStr"/>
+      <c r="E72" s="24" t="inlineStr"/>
+      <c r="F72" s="24" t="inlineStr"/>
+      <c r="G72" s="24" t="inlineStr"/>
+      <c r="H72" s="24" t="inlineStr"/>
+      <c r="I72" s="24" t="inlineStr"/>
+      <c r="J72" s="24" t="inlineStr"/>
+      <c r="K72" s="24" t="inlineStr"/>
+      <c r="L72" s="24" t="inlineStr"/>
+      <c r="M72" s="27" t="inlineStr"/>
       <c r="N72" s="1" t="n"/>
       <c r="O72" s="1" t="n"/>
       <c r="P72" s="1" t="n"/>
@@ -4017,16 +3977,16 @@
           <t>1914</t>
         </is>
       </c>
-      <c r="D73" s="24" t="n"/>
-      <c r="E73" s="24" t="n"/>
-      <c r="F73" s="24" t="n"/>
-      <c r="G73" s="24" t="n"/>
-      <c r="H73" s="24" t="n"/>
-      <c r="I73" s="24" t="n"/>
-      <c r="J73" s="24" t="n"/>
-      <c r="K73" s="24" t="n"/>
-      <c r="L73" s="24" t="n"/>
-      <c r="M73" s="27" t="n"/>
+      <c r="D73" s="24" t="inlineStr"/>
+      <c r="E73" s="24" t="inlineStr"/>
+      <c r="F73" s="24" t="inlineStr"/>
+      <c r="G73" s="24" t="inlineStr"/>
+      <c r="H73" s="24" t="inlineStr"/>
+      <c r="I73" s="24" t="inlineStr"/>
+      <c r="J73" s="24" t="inlineStr"/>
+      <c r="K73" s="24" t="inlineStr"/>
+      <c r="L73" s="24" t="inlineStr"/>
+      <c r="M73" s="27" t="inlineStr"/>
       <c r="N73" s="1" t="n"/>
       <c r="O73" s="1" t="n"/>
       <c r="P73" s="1" t="n"/>
@@ -4062,16 +4022,16 @@
           <t>1915</t>
         </is>
       </c>
-      <c r="D74" s="24" t="n"/>
-      <c r="E74" s="24" t="n"/>
-      <c r="F74" s="24" t="n"/>
-      <c r="G74" s="24" t="n"/>
-      <c r="H74" s="24" t="n"/>
-      <c r="I74" s="24" t="n"/>
-      <c r="J74" s="24" t="n"/>
-      <c r="K74" s="24" t="n"/>
-      <c r="L74" s="24" t="n"/>
-      <c r="M74" s="27" t="n"/>
+      <c r="D74" s="24" t="inlineStr"/>
+      <c r="E74" s="24" t="inlineStr"/>
+      <c r="F74" s="24" t="inlineStr"/>
+      <c r="G74" s="24" t="inlineStr"/>
+      <c r="H74" s="24" t="inlineStr"/>
+      <c r="I74" s="24" t="inlineStr"/>
+      <c r="J74" s="24" t="inlineStr"/>
+      <c r="K74" s="24" t="inlineStr"/>
+      <c r="L74" s="24" t="inlineStr"/>
+      <c r="M74" s="27" t="inlineStr"/>
       <c r="N74" s="1" t="n"/>
       <c r="O74" s="1" t="n"/>
       <c r="P74" s="1" t="n"/>
@@ -4107,16 +4067,16 @@
           <t>1916</t>
         </is>
       </c>
-      <c r="D75" s="24" t="n"/>
-      <c r="E75" s="24" t="n"/>
-      <c r="F75" s="24" t="n"/>
-      <c r="G75" s="24" t="n"/>
-      <c r="H75" s="24" t="n"/>
-      <c r="I75" s="24" t="n"/>
-      <c r="J75" s="24" t="n"/>
-      <c r="K75" s="24" t="n"/>
-      <c r="L75" s="24" t="n"/>
-      <c r="M75" s="27" t="n"/>
+      <c r="D75" s="24" t="inlineStr"/>
+      <c r="E75" s="24" t="inlineStr"/>
+      <c r="F75" s="24" t="inlineStr"/>
+      <c r="G75" s="24" t="inlineStr"/>
+      <c r="H75" s="24" t="inlineStr"/>
+      <c r="I75" s="24" t="inlineStr"/>
+      <c r="J75" s="24" t="inlineStr"/>
+      <c r="K75" s="24" t="inlineStr"/>
+      <c r="L75" s="24" t="inlineStr"/>
+      <c r="M75" s="27" t="inlineStr"/>
       <c r="N75" s="1" t="n"/>
       <c r="O75" s="1" t="n"/>
       <c r="P75" s="1" t="n"/>
@@ -4152,16 +4112,16 @@
           <t>1916</t>
         </is>
       </c>
-      <c r="D76" s="24" t="n"/>
-      <c r="E76" s="24" t="n"/>
-      <c r="F76" s="24" t="n"/>
-      <c r="G76" s="24" t="n"/>
-      <c r="H76" s="24" t="n"/>
-      <c r="I76" s="24" t="n"/>
-      <c r="J76" s="24" t="n"/>
-      <c r="K76" s="24" t="n"/>
-      <c r="L76" s="24" t="n"/>
-      <c r="M76" s="27" t="n"/>
+      <c r="D76" s="24" t="inlineStr"/>
+      <c r="E76" s="24" t="inlineStr"/>
+      <c r="F76" s="24" t="inlineStr"/>
+      <c r="G76" s="24" t="inlineStr"/>
+      <c r="H76" s="24" t="inlineStr"/>
+      <c r="I76" s="24" t="inlineStr"/>
+      <c r="J76" s="24" t="inlineStr"/>
+      <c r="K76" s="24" t="inlineStr"/>
+      <c r="L76" s="24" t="inlineStr"/>
+      <c r="M76" s="27" t="inlineStr"/>
       <c r="N76" s="1" t="n"/>
       <c r="O76" s="1" t="n"/>
       <c r="P76" s="1" t="n"/>
@@ -4197,16 +4157,16 @@
           <t>1918–1921</t>
         </is>
       </c>
-      <c r="D77" s="24" t="n"/>
-      <c r="E77" s="24" t="n"/>
-      <c r="F77" s="24" t="n"/>
-      <c r="G77" s="24" t="n"/>
-      <c r="H77" s="24" t="n"/>
-      <c r="I77" s="24" t="n"/>
-      <c r="J77" s="24" t="n"/>
-      <c r="K77" s="24" t="n"/>
-      <c r="L77" s="24" t="n"/>
-      <c r="M77" s="27" t="n"/>
+      <c r="D77" s="24" t="inlineStr"/>
+      <c r="E77" s="24" t="inlineStr"/>
+      <c r="F77" s="24" t="inlineStr"/>
+      <c r="G77" s="24" t="inlineStr"/>
+      <c r="H77" s="24" t="inlineStr"/>
+      <c r="I77" s="24" t="inlineStr"/>
+      <c r="J77" s="24" t="inlineStr"/>
+      <c r="K77" s="24" t="inlineStr"/>
+      <c r="L77" s="24" t="inlineStr"/>
+      <c r="M77" s="27" t="inlineStr"/>
       <c r="N77" s="1" t="n"/>
       <c r="O77" s="1" t="n"/>
       <c r="P77" s="1" t="n"/>
@@ -4242,16 +4202,16 @@
           <t>1830–1867</t>
         </is>
       </c>
-      <c r="D78" s="24" t="n"/>
-      <c r="E78" s="24" t="n"/>
-      <c r="F78" s="24" t="n"/>
-      <c r="G78" s="24" t="n"/>
-      <c r="H78" s="24" t="n"/>
-      <c r="I78" s="24" t="n"/>
-      <c r="J78" s="24" t="n"/>
-      <c r="K78" s="24" t="n"/>
-      <c r="L78" s="24" t="n"/>
-      <c r="M78" s="27" t="n"/>
+      <c r="D78" s="24" t="inlineStr"/>
+      <c r="E78" s="24" t="inlineStr"/>
+      <c r="F78" s="24" t="inlineStr"/>
+      <c r="G78" s="24" t="inlineStr"/>
+      <c r="H78" s="24" t="inlineStr"/>
+      <c r="I78" s="24" t="inlineStr"/>
+      <c r="J78" s="24" t="inlineStr"/>
+      <c r="K78" s="24" t="inlineStr"/>
+      <c r="L78" s="24" t="inlineStr"/>
+      <c r="M78" s="27" t="inlineStr"/>
       <c r="N78" s="1" t="n"/>
       <c r="O78" s="1" t="n"/>
       <c r="P78" s="1" t="n"/>
@@ -4287,16 +4247,16 @@
           <t>1800–1913</t>
         </is>
       </c>
-      <c r="D79" s="24" t="n"/>
-      <c r="E79" s="24" t="n"/>
-      <c r="F79" s="24" t="n"/>
-      <c r="G79" s="24" t="n"/>
-      <c r="H79" s="24" t="n"/>
-      <c r="I79" s="24" t="n"/>
-      <c r="J79" s="24" t="n"/>
-      <c r="K79" s="24" t="n"/>
-      <c r="L79" s="24" t="n"/>
-      <c r="M79" s="27" t="n"/>
+      <c r="D79" s="24" t="inlineStr"/>
+      <c r="E79" s="24" t="inlineStr"/>
+      <c r="F79" s="24" t="inlineStr"/>
+      <c r="G79" s="24" t="inlineStr"/>
+      <c r="H79" s="24" t="inlineStr"/>
+      <c r="I79" s="24" t="inlineStr"/>
+      <c r="J79" s="24" t="inlineStr"/>
+      <c r="K79" s="24" t="inlineStr"/>
+      <c r="L79" s="24" t="inlineStr"/>
+      <c r="M79" s="27" t="inlineStr"/>
       <c r="N79" s="1" t="n"/>
       <c r="O79" s="1" t="n"/>
       <c r="P79" s="1" t="n"/>
@@ -4332,16 +4292,16 @@
           <t>1739–1913</t>
         </is>
       </c>
-      <c r="D80" s="24" t="n"/>
-      <c r="E80" s="24" t="n"/>
-      <c r="F80" s="24" t="n"/>
-      <c r="G80" s="24" t="n"/>
-      <c r="H80" s="24" t="n"/>
-      <c r="I80" s="24" t="n"/>
-      <c r="J80" s="24" t="n"/>
-      <c r="K80" s="24" t="n"/>
-      <c r="L80" s="24" t="n"/>
-      <c r="M80" s="27" t="n"/>
+      <c r="D80" s="24" t="inlineStr"/>
+      <c r="E80" s="24" t="inlineStr"/>
+      <c r="F80" s="24" t="inlineStr"/>
+      <c r="G80" s="24" t="inlineStr"/>
+      <c r="H80" s="24" t="inlineStr"/>
+      <c r="I80" s="24" t="inlineStr"/>
+      <c r="J80" s="24" t="inlineStr"/>
+      <c r="K80" s="24" t="inlineStr"/>
+      <c r="L80" s="24" t="inlineStr"/>
+      <c r="M80" s="27" t="inlineStr"/>
       <c r="N80" s="1" t="n"/>
       <c r="O80" s="1" t="n"/>
       <c r="P80" s="1" t="n"/>
@@ -4377,16 +4337,16 @@
           <t>1796–1913</t>
         </is>
       </c>
-      <c r="D81" s="24" t="n"/>
-      <c r="E81" s="24" t="n"/>
-      <c r="F81" s="24" t="n"/>
-      <c r="G81" s="24" t="n"/>
-      <c r="H81" s="24" t="n"/>
-      <c r="I81" s="24" t="n"/>
-      <c r="J81" s="24" t="n"/>
-      <c r="K81" s="24" t="n"/>
-      <c r="L81" s="24" t="n"/>
-      <c r="M81" s="27" t="n"/>
+      <c r="D81" s="24" t="inlineStr"/>
+      <c r="E81" s="24" t="inlineStr"/>
+      <c r="F81" s="24" t="inlineStr"/>
+      <c r="G81" s="24" t="inlineStr"/>
+      <c r="H81" s="24" t="inlineStr"/>
+      <c r="I81" s="24" t="inlineStr"/>
+      <c r="J81" s="24" t="inlineStr"/>
+      <c r="K81" s="24" t="inlineStr"/>
+      <c r="L81" s="24" t="inlineStr"/>
+      <c r="M81" s="27" t="inlineStr"/>
       <c r="N81" s="1" t="n"/>
       <c r="O81" s="1" t="n"/>
       <c r="P81" s="1" t="n"/>
@@ -4422,16 +4382,16 @@
           <t>1755–1896</t>
         </is>
       </c>
-      <c r="D82" s="24" t="n"/>
-      <c r="E82" s="24" t="n"/>
-      <c r="F82" s="24" t="n"/>
-      <c r="G82" s="24" t="n"/>
-      <c r="H82" s="24" t="n"/>
-      <c r="I82" s="24" t="n"/>
-      <c r="J82" s="24" t="n"/>
-      <c r="K82" s="24" t="n"/>
-      <c r="L82" s="24" t="n"/>
-      <c r="M82" s="27" t="n"/>
+      <c r="D82" s="24" t="inlineStr"/>
+      <c r="E82" s="24" t="inlineStr"/>
+      <c r="F82" s="24" t="inlineStr"/>
+      <c r="G82" s="24" t="inlineStr"/>
+      <c r="H82" s="24" t="inlineStr"/>
+      <c r="I82" s="24" t="inlineStr"/>
+      <c r="J82" s="24" t="inlineStr"/>
+      <c r="K82" s="24" t="inlineStr"/>
+      <c r="L82" s="24" t="inlineStr"/>
+      <c r="M82" s="27" t="inlineStr"/>
       <c r="N82" s="1" t="n"/>
       <c r="O82" s="1" t="n"/>
       <c r="P82" s="1" t="n"/>
@@ -4467,16 +4427,16 @@
           <t>1869–1922</t>
         </is>
       </c>
-      <c r="D83" s="24" t="n"/>
-      <c r="E83" s="24" t="n"/>
-      <c r="F83" s="24" t="n"/>
-      <c r="G83" s="24" t="n"/>
-      <c r="H83" s="24" t="n"/>
-      <c r="I83" s="24" t="n"/>
-      <c r="J83" s="24" t="n"/>
-      <c r="K83" s="24" t="n"/>
-      <c r="L83" s="24" t="n"/>
-      <c r="M83" s="27" t="n"/>
+      <c r="D83" s="24" t="inlineStr"/>
+      <c r="E83" s="24" t="inlineStr"/>
+      <c r="F83" s="24" t="inlineStr"/>
+      <c r="G83" s="24" t="inlineStr"/>
+      <c r="H83" s="24" t="inlineStr"/>
+      <c r="I83" s="24" t="inlineStr"/>
+      <c r="J83" s="24" t="inlineStr"/>
+      <c r="K83" s="24" t="inlineStr"/>
+      <c r="L83" s="24" t="inlineStr"/>
+      <c r="M83" s="27" t="inlineStr"/>
       <c r="N83" s="1" t="n"/>
       <c r="O83" s="1" t="n"/>
       <c r="P83" s="1" t="n"/>
@@ -4512,16 +4472,16 @@
           <t>1782, 1795–1917</t>
         </is>
       </c>
-      <c r="D84" s="24" t="n"/>
-      <c r="E84" s="24" t="n"/>
-      <c r="F84" s="24" t="n"/>
-      <c r="G84" s="24" t="n"/>
-      <c r="H84" s="24" t="n"/>
-      <c r="I84" s="24" t="n"/>
-      <c r="J84" s="24" t="n"/>
-      <c r="K84" s="24" t="n"/>
-      <c r="L84" s="24" t="n"/>
-      <c r="M84" s="27" t="n"/>
+      <c r="D84" s="24" t="inlineStr"/>
+      <c r="E84" s="24" t="inlineStr"/>
+      <c r="F84" s="24" t="inlineStr"/>
+      <c r="G84" s="24" t="inlineStr"/>
+      <c r="H84" s="24" t="inlineStr"/>
+      <c r="I84" s="24" t="inlineStr"/>
+      <c r="J84" s="24" t="inlineStr"/>
+      <c r="K84" s="24" t="inlineStr"/>
+      <c r="L84" s="24" t="inlineStr"/>
+      <c r="M84" s="27" t="inlineStr"/>
       <c r="N84" s="1" t="n"/>
       <c r="O84" s="1" t="n"/>
       <c r="P84" s="1" t="n"/>
@@ -4557,16 +4517,16 @@
           <t>1897</t>
         </is>
       </c>
-      <c r="D85" s="24" t="n"/>
-      <c r="E85" s="24" t="n"/>
-      <c r="F85" s="24" t="n"/>
-      <c r="G85" s="24" t="n"/>
-      <c r="H85" s="24" t="n"/>
-      <c r="I85" s="24" t="n"/>
-      <c r="J85" s="24" t="n"/>
-      <c r="K85" s="24" t="n"/>
-      <c r="L85" s="24" t="n"/>
-      <c r="M85" s="27" t="n"/>
+      <c r="D85" s="24" t="inlineStr"/>
+      <c r="E85" s="24" t="inlineStr"/>
+      <c r="F85" s="24" t="inlineStr"/>
+      <c r="G85" s="24" t="inlineStr"/>
+      <c r="H85" s="24" t="inlineStr"/>
+      <c r="I85" s="24" t="inlineStr"/>
+      <c r="J85" s="24" t="inlineStr"/>
+      <c r="K85" s="24" t="inlineStr"/>
+      <c r="L85" s="24" t="inlineStr"/>
+      <c r="M85" s="27" t="inlineStr"/>
       <c r="N85" s="1" t="n"/>
       <c r="O85" s="1" t="n"/>
       <c r="P85" s="1" t="n"/>
@@ -4602,16 +4562,16 @@
           <t>1798–1876</t>
         </is>
       </c>
-      <c r="D86" s="24" t="n"/>
-      <c r="E86" s="24" t="n"/>
-      <c r="F86" s="24" t="n"/>
-      <c r="G86" s="24" t="n"/>
-      <c r="H86" s="24" t="n"/>
-      <c r="I86" s="24" t="n"/>
-      <c r="J86" s="24" t="n"/>
-      <c r="K86" s="24" t="n"/>
-      <c r="L86" s="24" t="n"/>
-      <c r="M86" s="27" t="n"/>
+      <c r="D86" s="24" t="inlineStr"/>
+      <c r="E86" s="24" t="inlineStr"/>
+      <c r="F86" s="24" t="inlineStr"/>
+      <c r="G86" s="24" t="inlineStr"/>
+      <c r="H86" s="24" t="inlineStr"/>
+      <c r="I86" s="24" t="inlineStr"/>
+      <c r="J86" s="24" t="inlineStr"/>
+      <c r="K86" s="24" t="inlineStr"/>
+      <c r="L86" s="24" t="inlineStr"/>
+      <c r="M86" s="27" t="inlineStr"/>
       <c r="N86" s="1" t="n"/>
       <c r="O86" s="1" t="n"/>
       <c r="P86" s="1" t="n"/>
@@ -4647,16 +4607,16 @@
           <t>1758–1914</t>
         </is>
       </c>
-      <c r="D87" s="24" t="n"/>
-      <c r="E87" s="24" t="n"/>
-      <c r="F87" s="24" t="n"/>
-      <c r="G87" s="24" t="n"/>
-      <c r="H87" s="24" t="n"/>
-      <c r="I87" s="24" t="n"/>
-      <c r="J87" s="24" t="n"/>
-      <c r="K87" s="24" t="n"/>
-      <c r="L87" s="24" t="n"/>
-      <c r="M87" s="27" t="n"/>
+      <c r="D87" s="24" t="inlineStr"/>
+      <c r="E87" s="24" t="inlineStr"/>
+      <c r="F87" s="24" t="inlineStr"/>
+      <c r="G87" s="24" t="inlineStr"/>
+      <c r="H87" s="24" t="inlineStr"/>
+      <c r="I87" s="24" t="inlineStr"/>
+      <c r="J87" s="24" t="inlineStr"/>
+      <c r="K87" s="24" t="inlineStr"/>
+      <c r="L87" s="24" t="inlineStr"/>
+      <c r="M87" s="27" t="inlineStr"/>
       <c r="N87" s="1" t="n"/>
       <c r="O87" s="1" t="n"/>
       <c r="P87" s="1" t="n"/>
@@ -4692,16 +4652,16 @@
           <t>1797–1915</t>
         </is>
       </c>
-      <c r="D88" s="24" t="n"/>
-      <c r="E88" s="24" t="n"/>
-      <c r="F88" s="24" t="n"/>
-      <c r="G88" s="24" t="n"/>
-      <c r="H88" s="24" t="n"/>
-      <c r="I88" s="24" t="n"/>
-      <c r="J88" s="24" t="n"/>
-      <c r="K88" s="24" t="n"/>
-      <c r="L88" s="24" t="n"/>
-      <c r="M88" s="27" t="n"/>
+      <c r="D88" s="24" t="inlineStr"/>
+      <c r="E88" s="24" t="inlineStr"/>
+      <c r="F88" s="24" t="inlineStr"/>
+      <c r="G88" s="24" t="inlineStr"/>
+      <c r="H88" s="24" t="inlineStr"/>
+      <c r="I88" s="24" t="inlineStr"/>
+      <c r="J88" s="24" t="inlineStr"/>
+      <c r="K88" s="24" t="inlineStr"/>
+      <c r="L88" s="24" t="inlineStr"/>
+      <c r="M88" s="27" t="inlineStr"/>
       <c r="N88" s="1" t="n"/>
       <c r="O88" s="1" t="n"/>
       <c r="P88" s="1" t="n"/>
@@ -4737,16 +4697,16 @@
           <t>1730–1914</t>
         </is>
       </c>
-      <c r="D89" s="24" t="n"/>
-      <c r="E89" s="24" t="n"/>
-      <c r="F89" s="24" t="n"/>
-      <c r="G89" s="24" t="n"/>
-      <c r="H89" s="24" t="n"/>
-      <c r="I89" s="24" t="n"/>
-      <c r="J89" s="24" t="n"/>
-      <c r="K89" s="24" t="n"/>
-      <c r="L89" s="24" t="n"/>
-      <c r="M89" s="27" t="n"/>
+      <c r="D89" s="24" t="inlineStr"/>
+      <c r="E89" s="24" t="inlineStr"/>
+      <c r="F89" s="24" t="inlineStr"/>
+      <c r="G89" s="24" t="inlineStr"/>
+      <c r="H89" s="24" t="inlineStr"/>
+      <c r="I89" s="24" t="inlineStr"/>
+      <c r="J89" s="24" t="inlineStr"/>
+      <c r="K89" s="24" t="inlineStr"/>
+      <c r="L89" s="24" t="inlineStr"/>
+      <c r="M89" s="27" t="inlineStr"/>
       <c r="N89" s="1" t="n"/>
       <c r="O89" s="1" t="n"/>
       <c r="P89" s="1" t="n"/>
@@ -4782,16 +4742,16 @@
           <t>1730–1914</t>
         </is>
       </c>
-      <c r="D90" s="24" t="n"/>
-      <c r="E90" s="24" t="n"/>
-      <c r="F90" s="24" t="n"/>
-      <c r="G90" s="24" t="n"/>
-      <c r="H90" s="24" t="n"/>
-      <c r="I90" s="24" t="n"/>
-      <c r="J90" s="24" t="n"/>
-      <c r="K90" s="24" t="n"/>
-      <c r="L90" s="24" t="n"/>
-      <c r="M90" s="27" t="n"/>
+      <c r="D90" s="24" t="inlineStr"/>
+      <c r="E90" s="24" t="inlineStr"/>
+      <c r="F90" s="24" t="inlineStr"/>
+      <c r="G90" s="24" t="inlineStr"/>
+      <c r="H90" s="24" t="inlineStr"/>
+      <c r="I90" s="24" t="inlineStr"/>
+      <c r="J90" s="24" t="inlineStr"/>
+      <c r="K90" s="24" t="inlineStr"/>
+      <c r="L90" s="24" t="inlineStr"/>
+      <c r="M90" s="27" t="inlineStr"/>
       <c r="N90" s="1" t="n"/>
       <c r="O90" s="1" t="n"/>
       <c r="P90" s="1" t="n"/>
@@ -4827,16 +4787,16 @@
           <t>1822–1909</t>
         </is>
       </c>
-      <c r="D91" s="24" t="n"/>
-      <c r="E91" s="24" t="n"/>
-      <c r="F91" s="24" t="n"/>
-      <c r="G91" s="24" t="n"/>
-      <c r="H91" s="24" t="n"/>
-      <c r="I91" s="24" t="n"/>
-      <c r="J91" s="24" t="n"/>
-      <c r="K91" s="24" t="n"/>
-      <c r="L91" s="24" t="n"/>
-      <c r="M91" s="27" t="n"/>
+      <c r="D91" s="24" t="inlineStr"/>
+      <c r="E91" s="24" t="inlineStr"/>
+      <c r="F91" s="24" t="inlineStr"/>
+      <c r="G91" s="24" t="inlineStr"/>
+      <c r="H91" s="24" t="inlineStr"/>
+      <c r="I91" s="24" t="inlineStr"/>
+      <c r="J91" s="24" t="inlineStr"/>
+      <c r="K91" s="24" t="inlineStr"/>
+      <c r="L91" s="24" t="inlineStr"/>
+      <c r="M91" s="27" t="inlineStr"/>
       <c r="N91" s="1" t="n"/>
       <c r="O91" s="1" t="n"/>
       <c r="P91" s="1" t="n"/>
@@ -4872,16 +4832,16 @@
           <t>1807–1907</t>
         </is>
       </c>
-      <c r="D92" s="24" t="n"/>
-      <c r="E92" s="24" t="n"/>
-      <c r="F92" s="24" t="n"/>
-      <c r="G92" s="24" t="n"/>
-      <c r="H92" s="24" t="n"/>
-      <c r="I92" s="24" t="n"/>
-      <c r="J92" s="24" t="n"/>
-      <c r="K92" s="24" t="n"/>
-      <c r="L92" s="24" t="n"/>
-      <c r="M92" s="27" t="n"/>
+      <c r="D92" s="24" t="inlineStr"/>
+      <c r="E92" s="24" t="inlineStr"/>
+      <c r="F92" s="24" t="inlineStr"/>
+      <c r="G92" s="24" t="inlineStr"/>
+      <c r="H92" s="24" t="inlineStr"/>
+      <c r="I92" s="24" t="inlineStr"/>
+      <c r="J92" s="24" t="inlineStr"/>
+      <c r="K92" s="24" t="inlineStr"/>
+      <c r="L92" s="24" t="inlineStr"/>
+      <c r="M92" s="27" t="inlineStr"/>
       <c r="N92" s="1" t="n"/>
       <c r="O92" s="1" t="n"/>
       <c r="P92" s="1" t="n"/>
@@ -4917,16 +4877,16 @@
           <t>1796–1879</t>
         </is>
       </c>
-      <c r="D93" s="24" t="n"/>
-      <c r="E93" s="24" t="n"/>
-      <c r="F93" s="24" t="n"/>
-      <c r="G93" s="24" t="n"/>
-      <c r="H93" s="24" t="n"/>
-      <c r="I93" s="24" t="n"/>
-      <c r="J93" s="24" t="n"/>
-      <c r="K93" s="24" t="n"/>
-      <c r="L93" s="24" t="n"/>
-      <c r="M93" s="27" t="n"/>
+      <c r="D93" s="24" t="inlineStr"/>
+      <c r="E93" s="24" t="inlineStr"/>
+      <c r="F93" s="24" t="inlineStr"/>
+      <c r="G93" s="24" t="inlineStr"/>
+      <c r="H93" s="24" t="inlineStr"/>
+      <c r="I93" s="24" t="inlineStr"/>
+      <c r="J93" s="24" t="inlineStr"/>
+      <c r="K93" s="24" t="inlineStr"/>
+      <c r="L93" s="24" t="inlineStr"/>
+      <c r="M93" s="27" t="inlineStr"/>
       <c r="N93" s="1" t="n"/>
       <c r="O93" s="1" t="n"/>
       <c r="P93" s="1" t="n"/>
@@ -4962,16 +4922,16 @@
           <t>1803–1877</t>
         </is>
       </c>
-      <c r="D94" s="24" t="n"/>
-      <c r="E94" s="24" t="n"/>
-      <c r="F94" s="24" t="n"/>
-      <c r="G94" s="24" t="n"/>
-      <c r="H94" s="24" t="n"/>
-      <c r="I94" s="24" t="n"/>
-      <c r="J94" s="24" t="n"/>
-      <c r="K94" s="24" t="n"/>
-      <c r="L94" s="24" t="n"/>
-      <c r="M94" s="27" t="n"/>
+      <c r="D94" s="24" t="inlineStr"/>
+      <c r="E94" s="24" t="inlineStr"/>
+      <c r="F94" s="24" t="inlineStr"/>
+      <c r="G94" s="24" t="inlineStr"/>
+      <c r="H94" s="24" t="inlineStr"/>
+      <c r="I94" s="24" t="inlineStr"/>
+      <c r="J94" s="24" t="inlineStr"/>
+      <c r="K94" s="24" t="inlineStr"/>
+      <c r="L94" s="24" t="inlineStr"/>
+      <c r="M94" s="27" t="inlineStr"/>
       <c r="N94" s="1" t="n"/>
       <c r="O94" s="1" t="n"/>
       <c r="P94" s="1" t="n"/>
@@ -5007,16 +4967,16 @@
           <t>1805–1910</t>
         </is>
       </c>
-      <c r="D95" s="24" t="n"/>
-      <c r="E95" s="24" t="n"/>
-      <c r="F95" s="24" t="n"/>
-      <c r="G95" s="24" t="n"/>
-      <c r="H95" s="24" t="n"/>
-      <c r="I95" s="24" t="n"/>
-      <c r="J95" s="24" t="n"/>
-      <c r="K95" s="24" t="n"/>
-      <c r="L95" s="24" t="n"/>
-      <c r="M95" s="27" t="n"/>
+      <c r="D95" s="24" t="inlineStr"/>
+      <c r="E95" s="24" t="inlineStr"/>
+      <c r="F95" s="24" t="inlineStr"/>
+      <c r="G95" s="24" t="inlineStr"/>
+      <c r="H95" s="24" t="inlineStr"/>
+      <c r="I95" s="24" t="inlineStr"/>
+      <c r="J95" s="24" t="inlineStr"/>
+      <c r="K95" s="24" t="inlineStr"/>
+      <c r="L95" s="24" t="inlineStr"/>
+      <c r="M95" s="27" t="inlineStr"/>
       <c r="N95" s="1" t="n"/>
       <c r="O95" s="1" t="n"/>
       <c r="P95" s="1" t="n"/>
@@ -5052,16 +5012,16 @@
           <t>1799–1892</t>
         </is>
       </c>
-      <c r="D96" s="24" t="n"/>
-      <c r="E96" s="24" t="n"/>
-      <c r="F96" s="24" t="n"/>
-      <c r="G96" s="24" t="n"/>
-      <c r="H96" s="24" t="n"/>
-      <c r="I96" s="24" t="n"/>
-      <c r="J96" s="24" t="n"/>
-      <c r="K96" s="24" t="n"/>
-      <c r="L96" s="24" t="n"/>
-      <c r="M96" s="27" t="n"/>
+      <c r="D96" s="24" t="inlineStr"/>
+      <c r="E96" s="24" t="inlineStr"/>
+      <c r="F96" s="24" t="inlineStr"/>
+      <c r="G96" s="24" t="inlineStr"/>
+      <c r="H96" s="24" t="inlineStr"/>
+      <c r="I96" s="24" t="inlineStr"/>
+      <c r="J96" s="24" t="inlineStr"/>
+      <c r="K96" s="24" t="inlineStr"/>
+      <c r="L96" s="24" t="inlineStr"/>
+      <c r="M96" s="27" t="inlineStr"/>
       <c r="N96" s="1" t="n"/>
       <c r="O96" s="1" t="n"/>
       <c r="P96" s="1" t="n"/>
@@ -5097,16 +5057,16 @@
           <t>1772–1916</t>
         </is>
       </c>
-      <c r="D97" s="24" t="n"/>
-      <c r="E97" s="24" t="n"/>
-      <c r="F97" s="24" t="n"/>
-      <c r="G97" s="24" t="n"/>
-      <c r="H97" s="24" t="n"/>
-      <c r="I97" s="24" t="n"/>
-      <c r="J97" s="24" t="n"/>
-      <c r="K97" s="24" t="n"/>
-      <c r="L97" s="24" t="n"/>
-      <c r="M97" s="27" t="n"/>
+      <c r="D97" s="24" t="inlineStr"/>
+      <c r="E97" s="24" t="inlineStr"/>
+      <c r="F97" s="24" t="inlineStr"/>
+      <c r="G97" s="24" t="inlineStr"/>
+      <c r="H97" s="24" t="inlineStr"/>
+      <c r="I97" s="24" t="inlineStr"/>
+      <c r="J97" s="24" t="inlineStr"/>
+      <c r="K97" s="24" t="inlineStr"/>
+      <c r="L97" s="24" t="inlineStr"/>
+      <c r="M97" s="27" t="inlineStr"/>
       <c r="N97" s="1" t="n"/>
       <c r="O97" s="1" t="n"/>
       <c r="P97" s="1" t="n"/>

</xml_diff>

<commit_message>
change cache structure to one cache item per page version
</commit_message>
<xml_diff>
--- a/test/resources/unittest_DAZHO_1.xlsx
+++ b/test/resources/unittest_DAZHO_1.xlsx
@@ -1134,7 +1134,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>Decrees, reports, reports of the spiritual consistory, request, communication of church ministers. Diocese of church lands diocese</t>
+          <t>Decrees, reports, a message of spiritual consistory, requests, communication of church ministers. Diocese of church lands diocese</t>
         </is>
       </c>
       <c r="C10" s="25" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B21" s="5" t="inlineStr">
         <is>
-          <t>Decrees, disposal of spiritual consistory, business cases in the diocesan administration, cases of church lands. The case of the construction and repair of churches in the Volyn Diocese. Decrees of the Synod, the Senate, the order of the Consistory. Reports, the message of spiritual boards. Deed23 on official activity and clergy behavior</t>
+          <t>Decrees, disposal of spiritual consistory, financial state cases in the diocesan administration, cases of church lands. The case of the construction and repair of churches in the Volyn Diocese. Decrees of the Synod, the Senate, the order of the Consistory. Reports, the message of spiritual boards. Deed23 on official activity and clergy behavior</t>
         </is>
       </c>
       <c r="C21" s="25" t="inlineStr">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="B22" s="5" t="inlineStr">
         <is>
-          <t>Decrees, disposal of spiritual consistory, business cases in the diocesan administration, cases of church lands. The case of the construction and repair of churches in the Volyn Diocese. Decrees of the Synod, the Senate, the order of the Consistory. Reports, the message of spiritual boards. DEPARTMENTS ABOUT COLLECTIONS AND CULSIFIALS</t>
+          <t>Decrees, disposal of spiritual consistory, financial state cases in the diocesan administration, cases of church lands. The case of the construction and repair of churches in the Volyn Diocese. Decrees of the Synod, the Senate, the order of the Consistory. Reports, the message of spiritual boards. DEPARTMENTS ABOUT COLLECTIVE ACTIVITIES AND PUPILS</t>
         </is>
       </c>
       <c r="C22" s="25" t="inlineStr">
@@ -1944,7 +1944,7 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. The case of the founding of the Kremenets Epiphany Feast of the Nikolaev Brotherhood (c. 33)</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. The case of the foundation of the Kremenets Epiphany Feast of the Nikolaev Brotherhood (c. 33)</t>
         </is>
       </c>
       <c r="C28" s="25" t="inlineStr">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="B38" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. On the issuance of metric certificates. About the purpose, moving, awarding and dismissal of priests. Case of Persons annexed to Orthodoxy in 1903 (Ref. 104)</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. Cases of official activity and behavior of the clergy. About church lands. On the issuance of metric certificates. About the purpose, movement, awarding and dismissal of priests. Case of Persons annexed to Orthodoxy in 1903 (Ref. 104)</t>
         </is>
       </c>
       <c r="C38" s="25" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>Cases about the appointment, movement and release of church ministers. Cases about the issuance of metric certificates, adoption, termination of marriage</t>
+          <t>Cases about the appointment, movement and release of church ministers. Cases of Issuing Metric Certificates, Adoption, Division of Marriages</t>
         </is>
       </c>
       <c r="C43" s="25" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="B44" s="5" t="inlineStr">
         <is>
-          <t>Decrees of the Synod, the Senate, the order of the Consistory. DEPARTMENTS ABOUT COLLECTIONS AND CULSE</t>
+          <t>Decrees of the Synod, the Senate, the order of the Consistory. DEPARTMENTS ABOUT COLLECTIONS AND CULSIFIALS</t>
         </is>
       </c>
       <c r="C44" s="25" t="inlineStr">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="B72" s="5" t="inlineStr">
         <is>
-          <t>On the issuance of powers to the courts in courts of claim for the seizure of joint lands, felling of church forests, grass of fields and pastures, etc. The cases of peasants' complaints about priests and clergymen for the devastation of church forests. Cases on the exchange of church and peasant lands, leasing plots of church land. About the construction and repair of churches, the removal of places for new cemeteries and the expansion of existing cemeteries. On the opening of independent parishes. The case of repair and painting of the Cathedral Church in Starokostiantyniv (c. 117). On granting permits for the construction of roadside crosses and monuments. The case of a donation of Countess AA Grabbe Pochaevskaya Lavra sections of land for the construction of a monument temple (ref. 22). About donations by peasants with. Gladkovichi Ovruch County of Earth in X. Buda Lyar Ovruch St. Basil Monastery (Ref. 33)</t>
+          <t>On the issuance of powers to the courts in courts of claim for the seizure of joint lands, felling of church forests, grass of fields and pastures, etc. The cases of peasants' complaints about priests and clergymen for the devastation of church forests. Cases on the exchange of church and peasant lands, leasing plots of church land. About the construction and repair of churches, the removal of places for new cemeteries and the expansion of existing cemeteries. On the opening of independent parishes. The case of repair and painting of the Cathedral Church in Starokostiantyniv (c. 117). On granting permits for the construction of roadside crosses and monuments. The case of a donation of Countess AA Grabbe Pochayiv Lavra sections of land for the construction of a monument temple (ref. 22). About donations by peasants with. Gladkovichi Ovruch County of Earth in X. Buda Lyar Ovruch St. Basil Monastery (Ref. 33)</t>
         </is>
       </c>
       <c r="C72" s="25" t="inlineStr">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="B74" s="5" t="inlineStr">
         <is>
-          <t>On the issuance of powers to the courts in courts of claim for the seizure of joint lands, felling of church forests, grass of fields and pastures, etc. The cases of peasants' complaints about priests and clergymen for the devastation of church forests. Cases on the exchange of church and peasant lands, leasing plots of church land. About the construction and repair of churches, the removal of places for new cemeteries and the expansion of existing cemeteries. Cases for the opening of independent parishes in the diocese. About permission to arrange in Zhytomyr Lazaret "names of students of church schools of the Volyn Diocese" (Spr. 9). The case of antiquity monuments is destroyed during the fighting (Ref. 40). About setting the amount of losses from hostilities in the diocese (Ref. 73)</t>
+          <t>On the issuance of powers to the courts in courts of claim for the seizure of joint lands, felling of church forests, grass of fields and pastures, etc. The cases of peasants' complaints about priests and clergymen for the devastation of church forests. Cases on the exchange of church and peasant lands, leasing plots of church land. About the construction and repair of churches, the removal of places for new cemeteries and the expansion of existing cemeteries. Cases for the opening of independent parishes in the diocese. About permission to arrange in Zhytomyr Lazaret "names of students of church schools of the Volyn Diocese" (file 9). The case of antiquity monuments is destroyed during the fighting (Ref. 40). About setting the amount of losses from hostilities in the diocese (Ref. 73)</t>
         </is>
       </c>
       <c r="C74" s="25" t="inlineStr">

</xml_diff>